<commit_message>
added new print request
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="38">
   <si>
     <t>Date Requested</t>
   </si>
@@ -110,10 +110,10 @@
     <t>PLA</t>
   </si>
   <si>
-    <t>USB port mounting </t>
-  </si>
-  <si>
-    <t>wire twister2   </t>
+    <t>USB port mounting</t>
+  </si>
+  <si>
+    <t>wire twister2</t>
   </si>
   <si>
     <t>23-05-2018</t>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>connect block</t>
+  </si>
+  <si>
+    <t>Azad</t>
+  </si>
+  <si>
+    <t>Stethescopes</t>
   </si>
 </sst>
 </file>
@@ -241,12 +247,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -746,6 +752,7 @@
       <c r="A16" s="3" t="n">
         <v>43242</v>
       </c>
+      <c r="B16" s="0"/>
       <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
@@ -832,6 +839,35 @@
         <v>0.2</v>
       </c>
       <c r="J18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RV model will be done at end of day
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="38">
   <si>
     <t>Date Requested</t>
   </si>
@@ -86,6 +86,9 @@
     <t>LVAD RA</t>
   </si>
   <si>
+    <t>23-05-2018</t>
+  </si>
+  <si>
     <t>LVAD RV</t>
   </si>
   <si>
@@ -111,9 +114,6 @@
   </si>
   <si>
     <t>USB port mounting</t>
-  </si>
-  <si>
-    <t>23-05-2018</t>
   </si>
   <si>
     <t>wire twister2</t>
@@ -256,7 +256,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -562,16 +562,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B10" s="0"/>
+      <c r="B10" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>1</v>
@@ -600,16 +602,16 @@
         <v>43242</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G11" s="1" t="n">
         <v>2</v>
@@ -632,16 +634,16 @@
         <v>43242</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="G12" s="1" t="n">
         <v>2</v>
@@ -664,16 +666,16 @@
         <v>43242</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>2</v>
@@ -696,16 +698,16 @@
         <v>43242</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>2</v>
@@ -728,16 +730,16 @@
         <v>43242</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>2</v>
@@ -757,10 +759,10 @@
         <v>43242</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>33</v>
@@ -769,7 +771,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G16" s="1" t="n">
         <v>2</v>
@@ -789,10 +791,10 @@
         <v>43242</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>34</v>
@@ -801,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G17" s="1" t="n">
         <v>2</v>
@@ -824,7 +826,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>35</v>
@@ -833,7 +835,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G18" s="1" t="n">
         <v>2</v>
@@ -862,7 +864,7 @@
         <v>5</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G19" s="1" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
added new entries for prints for CAS
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="48">
   <si>
     <t>Date Requested</t>
   </si>
@@ -129,6 +129,36 @@
   </si>
   <si>
     <t>Stethescopes</t>
+  </si>
+  <si>
+    <t>24-05-2018</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>FOCUS a4c 100 scale</t>
+  </si>
+  <si>
+    <t>For CAS</t>
+  </si>
+  <si>
+    <t>FOCUS a4c 50 scale</t>
+  </si>
+  <si>
+    <t>FOCUS LAX 100 scale</t>
+  </si>
+  <si>
+    <t>FOCUS LAX 50 scale</t>
+  </si>
+  <si>
+    <t>FOCUS SAX 100 scale</t>
+  </si>
+  <si>
+    <t>FOCUS SAX 50 scale</t>
+  </si>
+  <si>
+    <t>Modular Bloodpool Model</t>
   </si>
 </sst>
 </file>
@@ -251,12 +281,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -882,6 +912,211 @@
         <v>13</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
updated the completed counts for several models
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC63CC92-83BA-4A04-BA76-520CE6EC7556}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="May 2018" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="May 2018" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="50">
   <si>
     <t>Date Requested</t>
   </si>
@@ -140,9 +146,6 @@
     <t>FOCUS a4c 100 scale</t>
   </si>
   <si>
-    <t>For CAS</t>
-  </si>
-  <si>
     <t>FOCUS a4c 50 scale</t>
   </si>
   <si>
@@ -159,17 +162,25 @@
   </si>
   <si>
     <t>Modular Bloodpool Model</t>
+  </si>
+  <si>
+    <t>6 complete</t>
+  </si>
+  <si>
+    <t>3 complete</t>
+  </si>
+  <si>
+    <t>0 complete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -178,22 +189,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -210,7 +206,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -218,93 +214,360 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK26"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.9311740890688"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.39676113360324"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1983805668016"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.27125506072875"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.3967611336032"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.1336032388664"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="13.53125" style="1"/>
+    <col min="3" max="3" width="9.06640625" style="1"/>
+    <col min="4" max="4" width="18.9296875" style="1"/>
+    <col min="5" max="5" width="11.46484375" style="1"/>
+    <col min="6" max="6" width="9.3984375" style="1"/>
+    <col min="7" max="7" width="12.19921875" style="1"/>
+    <col min="8" max="8" width="7.265625" style="1"/>
+    <col min="9" max="9" width="15.3984375" style="1"/>
+    <col min="10" max="10" width="9.53125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -336,11 +599,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" s="3">
         <v>43224</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="3">
         <v>43224</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -349,7 +612,7 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -361,18 +624,18 @@
       <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="I2" s="1">
         <v>0.1</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" s="3">
         <v>43224</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="3">
         <v>43225</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -381,7 +644,7 @@
       <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="1">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -393,18 +656,18 @@
       <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="I3" s="1">
         <v>0.1</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="3">
         <v>43224</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="3">
         <v>43225</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -413,7 +676,7 @@
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -425,18 +688,18 @@
       <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="1" t="n">
+      <c r="I4" s="1">
         <v>0.1</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" s="3">
         <v>43224</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="3">
         <v>43226</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -445,7 +708,7 @@
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -457,18 +720,18 @@
       <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="I5" s="1">
         <v>0.1</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="3">
         <v>43224</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="3">
         <v>43227</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -477,7 +740,7 @@
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -489,18 +752,18 @@
       <c r="H6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="1" t="n">
+      <c r="I6" s="1">
         <v>0.1</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="3">
         <v>43224</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="3">
         <v>43228</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -509,7 +772,7 @@
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -521,18 +784,18 @@
       <c r="H7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="1" t="n">
+      <c r="I7" s="1">
         <v>0.1</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="3">
         <v>43224</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="3">
         <v>43242</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -541,7 +804,7 @@
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -553,15 +816,15 @@
       <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="1" t="n">
+      <c r="I8" s="1">
         <v>0.1</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="3">
         <v>43224</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -573,7 +836,7 @@
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -585,15 +848,15 @@
       <c r="H9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="1" t="n">
+      <c r="I9" s="1">
         <v>0.1</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="3">
         <v>43224</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -605,7 +868,7 @@
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -617,18 +880,18 @@
       <c r="H10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="1" t="n">
+      <c r="I10" s="1">
         <v>0.1</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="3">
         <v>43238</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="3">
         <v>43242</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -637,30 +900,30 @@
       <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="1">
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I11" s="1" t="n">
+      <c r="G11" s="1">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1">
+        <v>20</v>
+      </c>
+      <c r="I11" s="1">
         <v>0.2</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="3">
         <v>43238</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="3">
         <v>43242</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -669,30 +932,30 @@
       <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="1">
         <v>2</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I12" s="1" t="n">
+      <c r="G12" s="1">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1">
+        <v>20</v>
+      </c>
+      <c r="I12" s="1">
         <v>0.2</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="3">
         <v>43238</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="3">
         <v>43242</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -701,30 +964,30 @@
       <c r="D13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="1">
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I13" s="1" t="n">
+      <c r="G13" s="1">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1">
+        <v>20</v>
+      </c>
+      <c r="I13" s="1">
         <v>0.2</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="3">
         <v>43238</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="3">
         <v>43242</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -733,30 +996,30 @@
       <c r="D14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="1">
         <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H14" s="1" t="n">
+      <c r="G14" s="1">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1">
         <v>100</v>
       </c>
-      <c r="I14" s="1" t="n">
+      <c r="I14" s="1">
         <v>0.2</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="3">
         <v>43238</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="3">
         <v>43242</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -765,27 +1028,27 @@
       <c r="D15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="1">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I15" s="1" t="n">
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1">
+        <v>20</v>
+      </c>
+      <c r="I15" s="1">
         <v>0.2</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="3">
         <v>43242</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -797,27 +1060,27 @@
       <c r="D16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="1">
         <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H16" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I16" s="1" t="n">
+      <c r="G16" s="1">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
+        <v>20</v>
+      </c>
+      <c r="I16" s="1">
         <v>0.2</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" s="3">
         <v>43242</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -829,27 +1092,27 @@
       <c r="D17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="1">
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I17" s="1" t="n">
+      <c r="G17" s="1">
+        <v>2</v>
+      </c>
+      <c r="H17" s="1">
+        <v>20</v>
+      </c>
+      <c r="I17" s="1">
         <v>0.2</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" s="3">
         <v>43242</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -861,26 +1124,26 @@
       <c r="D18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="1">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I18" s="1" t="n">
+      <c r="G18" s="1">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1">
+        <v>20</v>
+      </c>
+      <c r="I18" s="1">
         <v>0.2</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -893,26 +1156,26 @@
       <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="1">
         <v>5</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H19" s="1" t="n">
+      <c r="G19" s="1">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1">
         <v>100</v>
       </c>
-      <c r="I19" s="1" t="n">
+      <c r="I19" s="1">
         <v>0.2</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -922,26 +1185,26 @@
       <c r="D20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="1">
         <v>2</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H20" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I20" s="1" t="n">
+      <c r="G20" s="1">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1">
+        <v>20</v>
+      </c>
+      <c r="I20" s="1">
         <v>0.2</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -949,28 +1212,28 @@
         <v>39</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="E21" s="1">
         <v>21</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I21" s="1" t="n">
+      <c r="G21" s="1">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1">
+        <v>20</v>
+      </c>
+      <c r="I21" s="1">
         <v>0.2</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -978,28 +1241,28 @@
         <v>39</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="E22" s="1">
         <v>2</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I22" s="1" t="n">
+      <c r="G22" s="1">
+        <v>2</v>
+      </c>
+      <c r="H22" s="1">
+        <v>20</v>
+      </c>
+      <c r="I22" s="1">
         <v>0.2</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
@@ -1007,28 +1270,28 @@
         <v>39</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="E23" s="1">
         <v>21</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I23" s="1" t="n">
+      <c r="G23" s="1">
+        <v>2</v>
+      </c>
+      <c r="H23" s="1">
+        <v>20</v>
+      </c>
+      <c r="I23" s="1">
         <v>0.2</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
@@ -1036,28 +1299,28 @@
         <v>39</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="E24" s="1">
         <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H24" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I24" s="1" t="n">
+      <c r="G24" s="1">
+        <v>2</v>
+      </c>
+      <c r="H24" s="1">
+        <v>20</v>
+      </c>
+      <c r="I24" s="1">
         <v>0.2</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
@@ -1065,28 +1328,28 @@
         <v>39</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="E25" s="1">
         <v>21</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I25" s="1" t="n">
+      <c r="G25" s="1">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1">
+        <v>20</v>
+      </c>
+      <c r="I25" s="1">
         <v>0.2</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -1094,36 +1357,29 @@
         <v>39</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="E26" s="1">
         <v>10</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I26" s="1" t="n">
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1">
+        <v>20</v>
+      </c>
+      <c r="I26" s="1">
         <v>0.2</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated completed EVHP components
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
   <si>
     <t>Date Requested</t>
   </si>
@@ -149,7 +149,7 @@
     <t>FOCUS SAX 50 scale</t>
   </si>
   <si>
-    <t>7 complete</t>
+    <t>11 complete</t>
   </si>
   <si>
     <t>Modular Bloodpool Model</t>
@@ -158,10 +158,10 @@
     <t>25-05-2018</t>
   </si>
   <si>
+    <t>27-05-2018</t>
+  </si>
+  <si>
     <t>EVHP Holder Goose Neck to TEE Clip Adapter</t>
-  </si>
-  <si>
-    <t>26-05-2018</t>
   </si>
   <si>
     <t>EVHP Holder Goose Neck to Cannula Mount Adapter</t>
@@ -289,10 +289,10 @@
   </sheetPr>
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -864,6 +864,7 @@
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B20" s="0"/>
       <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
@@ -890,6 +891,7 @@
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B21" s="0"/>
       <c r="C21" s="1" t="s">
         <v>37</v>
       </c>
@@ -916,6 +918,7 @@
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B22" s="0"/>
       <c r="C22" s="1" t="s">
         <v>39</v>
       </c>
@@ -942,6 +945,7 @@
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B23" s="0"/>
       <c r="C23" s="1" t="s">
         <v>40</v>
       </c>
@@ -968,6 +972,7 @@
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B24" s="0"/>
       <c r="C24" s="1" t="s">
         <v>42</v>
       </c>
@@ -994,6 +999,7 @@
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B25" s="0"/>
       <c r="C25" s="1" t="s">
         <v>43</v>
       </c>
@@ -1020,6 +1026,7 @@
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B26" s="0"/>
       <c r="C26" s="1" t="s">
         <v>45</v>
       </c>
@@ -1046,8 +1053,11 @@
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="B27" s="0" t="s">
+        <v>47</v>
+      </c>
       <c r="C27" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>1</v>
@@ -1073,7 +1083,7 @@
         <v>46</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
added request for new TEE Spacer
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="52">
   <si>
     <t>Date Requested</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>EVHP Holder Goose Neck to Cannula Mount Adapter</t>
+  </si>
+  <si>
+    <t>TEE Spacer</t>
+  </si>
+  <si>
+    <t>Polyflex</t>
   </si>
 </sst>
 </file>
@@ -287,12 +293,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1049,11 +1055,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1104,6 +1110,35 @@
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated completion and target counts
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -131,7 +131,7 @@
     <t>FOCUS a4c 50 scale</t>
   </si>
   <si>
-    <t>12 complete</t>
+    <t>18 complete</t>
   </si>
   <si>
     <t>FOCUS LAX 100 scale</t>
@@ -298,7 +298,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
+      <selection pane="bottomLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -311,7 +311,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.53441295546559"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
   </cols>
   <sheetData>
@@ -902,7 +902,7 @@
         <v>37</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
@@ -947,7 +947,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -956,7 +956,7 @@
         <v>40</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>24</v>
@@ -1001,7 +1001,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>43</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
added new DORV request
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="54">
   <si>
     <t>Date Requested</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>Polyflex</t>
+  </si>
+  <si>
+    <t>29-05-2018</t>
+  </si>
+  <si>
+    <t>DORV #20</t>
   </si>
 </sst>
 </file>
@@ -293,12 +299,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1142,6 +1148,32 @@
         <v>11</v>
       </c>
     </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
updated DORV model completion
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
   <si>
     <t>Date Requested</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>29-05-2018</t>
+  </si>
+  <si>
+    <t>30-05-2018</t>
   </si>
   <si>
     <t>DORV #20</t>
@@ -301,10 +304,10 @@
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1152,8 +1155,11 @@
       <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="B30" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="C30" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
added new requests for ACHD models and updated counts for 50 scale models
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
   <si>
     <t>Date Requested</t>
   </si>
@@ -131,7 +131,7 @@
     <t>FOCUS a4c 50 scale</t>
   </si>
   <si>
-    <t>18 complete</t>
+    <t>24 complete</t>
   </si>
   <si>
     <t>FOCUS LAX 100 scale</t>
@@ -140,7 +140,7 @@
     <t>FOCUS LAX 50 scale</t>
   </si>
   <si>
-    <t>6 complete</t>
+    <t>12 complete</t>
   </si>
   <si>
     <t>FOCUS SAX 100 scale</t>
@@ -180,6 +180,15 @@
   </si>
   <si>
     <t>DORV #20</t>
+  </si>
+  <si>
+    <t>Full Fontan</t>
+  </si>
+  <si>
+    <t>Full Dextrocardia</t>
+  </si>
+  <si>
+    <t>Full TOF</t>
   </si>
 </sst>
 </file>
@@ -302,12 +311,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1180,6 +1189,84 @@
         <v>11</v>
       </c>
     </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
updated FOCUS SAX and LAX counts, added new request for tracheal rings
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="60">
   <si>
     <t>Date Requested</t>
   </si>
@@ -128,6 +128,9 @@
     <t>0 complete</t>
   </si>
   <si>
+    <t>30-05-2018</t>
+  </si>
+  <si>
     <t>FOCUS a4c 50 scale</t>
   </si>
   <si>
@@ -140,7 +143,7 @@
     <t>FOCUS LAX 50 scale</t>
   </si>
   <si>
-    <t>12 complete</t>
+    <t>18 complete</t>
   </si>
   <si>
     <t>FOCUS SAX 100 scale</t>
@@ -149,7 +152,7 @@
     <t>FOCUS SAX 50 scale</t>
   </si>
   <si>
-    <t>11 complete</t>
+    <t>15 complete</t>
   </si>
   <si>
     <t>Modular Bloodpool Model</t>
@@ -176,9 +179,6 @@
     <t>29-05-2018</t>
   </si>
   <si>
-    <t>30-05-2018</t>
-  </si>
-  <si>
     <t>DORV #20</t>
   </si>
   <si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>Full TOF</t>
+  </si>
+  <si>
+    <t>31-05-2018</t>
+  </si>
+  <si>
+    <t>Tracheal Rings</t>
   </si>
 </sst>
 </file>
@@ -311,12 +317,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+      <selection pane="bottomLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -911,13 +917,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="0"/>
+      <c r="B21" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>24</v>
@@ -935,7 +943,7 @@
         <v>0.2</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,7 +952,7 @@
       </c>
       <c r="B22" s="0"/>
       <c r="C22" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>2</v>
@@ -971,7 +979,7 @@
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>24</v>
@@ -989,7 +997,7 @@
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,7 +1006,7 @@
       </c>
       <c r="B24" s="0"/>
       <c r="C24" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>2</v>
@@ -1025,7 +1033,7 @@
       </c>
       <c r="B25" s="0"/>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>24</v>
@@ -1043,7 +1051,7 @@
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,7 +1060,7 @@
       </c>
       <c r="B26" s="0"/>
       <c r="C26" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>10</v>
@@ -1075,13 +1083,13 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>1</v>
@@ -1104,13 +1112,13 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>1</v>
@@ -1133,19 +1141,19 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F29" s="1" t="n">
         <v>1</v>
@@ -1162,10 +1170,10 @@
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>54</v>
@@ -1191,7 +1199,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>55</v>
@@ -1217,7 +1225,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>56</v>
@@ -1243,7 +1251,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>57</v>
@@ -1264,6 +1272,35 @@
         <v>0.2</v>
       </c>
       <c r="I33" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new requests for cable parts
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="68">
   <si>
     <t>Date Requested</t>
   </si>
@@ -212,6 +212,15 @@
   <si>
     <t>03-06-2018</t>
   </si>
+  <si>
+    <t>04-06-2018</t>
+  </si>
+  <si>
+    <t>Flow Cable End Clip</t>
+  </si>
+  <si>
+    <t>Flow Cable Fixing Block 2</t>
+  </si>
 </sst>
 </file>
 
@@ -1402,7 +1411,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10888,6 +10897,58 @@
         <v>11</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="1048553" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048554" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048555" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
updated completed evhp wire parts
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="68">
   <si>
     <t>Date Requested</t>
   </si>
@@ -1411,7 +1411,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10901,6 +10901,9 @@
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
@@ -10925,6 +10928,9 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C14" s="1" t="s">

</xml_diff>

<commit_message>
added request for more flow clips
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="69">
   <si>
     <t>Date Requested</t>
   </si>
@@ -221,6 +221,9 @@
   <si>
     <t>Flow Cable Fixing Block 2</t>
   </si>
+  <si>
+    <t>05-06-2018</t>
+  </si>
 </sst>
 </file>
 
@@ -1411,7 +1414,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10955,6 +10958,35 @@
         <v>11</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="1048553" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048554" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048555" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
new requests for EVHP parts
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="72">
   <si>
     <t>Date Requested</t>
   </si>
@@ -224,6 +224,15 @@
   <si>
     <t>05-06-2018</t>
   </si>
+  <si>
+    <t>08-06-2018</t>
+  </si>
+  <si>
+    <t>Press Cable End Clip</t>
+  </si>
+  <si>
+    <t>Flow Cable Fixing Block 3</t>
+  </si>
 </sst>
 </file>
 
@@ -350,7 +359,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+      <selection pane="bottomLeft" activeCell="A36" activeCellId="1" sqref="E17:I17 A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1411,10 +1420,10 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E17" activeCellId="0" sqref="E17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10987,6 +10996,58 @@
         <v>11</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="1048553" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048554" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048555" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
updated completion for more evhp prints
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="72">
   <si>
     <t>Date Requested</t>
   </si>
@@ -359,7 +359,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A36" activeCellId="1" sqref="E17:I17 A36"/>
+      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1420,10 +1420,10 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E17" activeCellId="0" sqref="E17:I17"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -11000,6 +11000,9 @@
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>70</v>
       </c>
@@ -11024,6 +11027,9 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C17" s="1" t="s">

</xml_diff>

<commit_message>
added requests for ultrasound probes and beams
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="75">
   <si>
     <t>Date Requested</t>
   </si>
@@ -233,6 +233,15 @@
   <si>
     <t>Flow Cable Fixing Block 3</t>
   </si>
+  <si>
+    <t>11-06-2018</t>
+  </si>
+  <si>
+    <t>75 scale tte probe</t>
+  </si>
+  <si>
+    <t>ultrasound beam 5x5 mm base</t>
+  </si>
 </sst>
 </file>
 
@@ -1421,9 +1430,9 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -11054,6 +11063,58 @@
         <v>11</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="1048553" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048554" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048555" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added requests for new EVHP funnels and TTE probes w/ultrasound beam planes
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="76">
   <si>
     <t>Date Requested</t>
   </si>
@@ -242,6 +242,9 @@
   <si>
     <t>ultrasound beam 5x5 mm base</t>
   </si>
+  <si>
+    <t>12-06-2018</t>
+  </si>
 </sst>
 </file>
 
@@ -1429,10 +1432,10 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -11071,7 +11074,7 @@
         <v>73</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
@@ -11097,7 +11100,7 @@
         <v>74</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>13</v>
@@ -11109,9 +11112,35 @@
         <v>11</v>
       </c>
       <c r="H19" s="1" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated completion counts for ultrasound beams
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="77">
   <si>
     <t>Date Requested</t>
   </si>
@@ -237,6 +237,9 @@
     <t>11-06-2018</t>
   </si>
   <si>
+    <t>13-06-2018</t>
+  </si>
+  <si>
     <t>75 scale tte probe</t>
   </si>
   <si>
@@ -369,7 +372,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
@@ -1432,10 +1435,10 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -11070,8 +11073,11 @@
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="B18" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>20</v>
@@ -11096,11 +11102,14 @@
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="B19" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>13</v>
@@ -11120,7 +11129,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
finished evhp funnel and evhp short TEE spacer
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="79">
   <si>
     <t>Date Requested</t>
   </si>
@@ -248,6 +248,12 @@
   <si>
     <t>12-06-2018</t>
   </si>
+  <si>
+    <t>18-06-2018</t>
+  </si>
+  <si>
+    <t>Short TEE Spacer</t>
+  </si>
 </sst>
 </file>
 
@@ -1433,15 +1439,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:65536"/>
+  <dimension ref="1:21"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.6"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
@@ -11131,6 +11137,9 @@
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>61</v>
       </c>
@@ -11153,30 +11162,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1048553" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
now preparing top verticies for chest reopening phantom frame
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="84">
   <si>
     <t>Date Requested</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>Rushil Printer Parts</t>
+  </si>
+  <si>
+    <t>21-06-2018</t>
+  </si>
+  <si>
+    <t>Chest Reopening Top Verticies</t>
+  </si>
+  <si>
+    <t>Polylite + PLA</t>
   </si>
 </sst>
 </file>
@@ -1450,12 +1459,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1464,7 +1473,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.0647773279352"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.39676113360324"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1619433198381"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
@@ -2096,6 +2105,32 @@
         <v>11</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
completion of chest reopening pieces
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="85">
   <si>
     <t>Date Requested</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>21-06-2018</t>
+  </si>
+  <si>
+    <t>22-06-2018</t>
   </si>
   <si>
     <t>Chest Reopening Top Verticies</t>
@@ -1464,7 +1467,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2109,14 +2112,17 @@
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="B23" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
request for 20 array tracheal rings
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ACDFE7-DB0B-4C97-9B44-4E04EE24DD6E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="May 2018" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="June 2018" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="May 2018" sheetId="1" r:id="rId1"/>
+    <sheet name="June 2018" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="87">
   <si>
     <t>Date Requested</t>
   </si>
@@ -271,18 +277,22 @@
   </si>
   <si>
     <t>Polylite + PLA</t>
+  </si>
+  <si>
+    <t>26-06-2018</t>
+  </si>
+  <si>
+    <t>Tracheal Rings od: 23.5 id: 15.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="DD/MMM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -291,22 +301,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -323,7 +318,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -331,96 +326,362 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK36"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.39676113360324"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="13.53125" style="1"/>
+    <col min="3" max="3" width="36.06640625" style="1"/>
+    <col min="4" max="4" width="11.46484375" style="1"/>
+    <col min="5" max="5" width="9.3984375" style="1"/>
+    <col min="6" max="6" width="12.19921875" style="1"/>
+    <col min="7" max="7" width="7.265625" style="1"/>
+    <col min="8" max="8" width="15.3984375" style="1"/>
+    <col min="9" max="9" width="11.46484375" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -449,17 +710,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="3">
         <v>43224</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="3">
         <v>43224</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -471,24 +732,24 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1">
         <v>0.1</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="3">
         <v>43224</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="3">
         <v>43225</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -500,24 +761,24 @@
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="1">
         <v>0.1</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="3">
         <v>43224</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="3">
         <v>43225</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -529,24 +790,24 @@
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="1">
         <v>0.1</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="3">
         <v>43224</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="3">
         <v>43226</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -558,24 +819,24 @@
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="1">
         <v>0.1</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="3">
         <v>43224</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="3">
         <v>43227</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -587,24 +848,24 @@
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="1">
         <v>0.1</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="3">
         <v>43224</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="3">
         <v>43228</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -616,24 +877,24 @@
       <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="1">
         <v>0.1</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="3">
         <v>43224</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="3">
         <v>43242</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -645,15 +906,15 @@
       <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="1">
         <v>0.1</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="3">
         <v>43224</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -662,7 +923,7 @@
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -674,15 +935,15 @@
       <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H9" s="1">
         <v>0.1</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="3">
         <v>43224</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -691,7 +952,7 @@
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -703,160 +964,160 @@
       <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="1">
         <v>0.1</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="3">
         <v>43238</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="3">
         <v>43242</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="3">
         <v>43238</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="3">
         <v>43242</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="3">
         <v>43238</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="3">
         <v>43242</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="3">
         <v>43238</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="3">
         <v>43242</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="n">
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
         <v>100</v>
       </c>
-      <c r="H14" s="1" t="n">
+      <c r="H14" s="1">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="3">
         <v>43238</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="3">
         <v>43242</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="3">
         <v>43242</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -865,27 +1126,27 @@
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1" t="n">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="3">
         <v>43242</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -894,27 +1155,27 @@
       <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1" t="n">
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="3">
         <v>43242</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -923,26 +1184,26 @@
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="n">
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -952,53 +1213,53 @@
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" s="1" t="n">
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
         <v>100</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="1">
         <v>0.2</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="0"/>
+      <c r="B20"/>
       <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="1">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="n">
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1">
         <v>0.2</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -1008,161 +1269,161 @@
       <c r="C21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="n">
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
         <v>0.2</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="0"/>
+      <c r="B22"/>
       <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="n">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="0"/>
+      <c r="B23"/>
       <c r="C23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="1">
         <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="n">
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="0"/>
+      <c r="B24"/>
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="1">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1" t="n">
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="0"/>
+      <c r="B25"/>
       <c r="C25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="1">
         <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1" t="n">
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="0"/>
+      <c r="B26"/>
       <c r="C26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="1">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1" t="n">
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1172,26 +1433,26 @@
       <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="1">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1" t="n">
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1201,26 +1462,26 @@
       <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="1">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1" t="n">
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -1230,26 +1491,26 @@
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1" t="n">
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
         <v>10</v>
       </c>
-      <c r="H29" s="1" t="n">
+      <c r="H29" s="1">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -1259,7 +1520,7 @@
       <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1271,95 +1532,95 @@
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="1" t="n">
+      <c r="H30" s="1">
         <v>0.2</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="0"/>
+      <c r="B31"/>
       <c r="C31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="D31" s="1">
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1" t="n">
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="0"/>
+      <c r="B32"/>
       <c r="C32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="1" t="n">
+      <c r="D32" s="1">
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G32" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H32" s="1" t="n">
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>20</v>
+      </c>
+      <c r="H32" s="1">
         <v>0.2</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="0"/>
+      <c r="B33"/>
       <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="1" t="n">
+      <c r="D33" s="1">
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H33" s="1" t="n">
+      <c r="F33" s="1">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1">
         <v>0.2</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -1369,26 +1630,26 @@
       <c r="C34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="1" t="n">
+      <c r="D34" s="1">
         <v>15</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G34" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H34" s="1" t="n">
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>20</v>
+      </c>
+      <c r="H34" s="1">
         <v>0.2</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
@@ -1398,26 +1659,26 @@
       <c r="C35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="1" t="n">
+      <c r="D35" s="1">
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H35" s="1" t="n">
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1">
         <v>0.2</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
@@ -1427,19 +1688,19 @@
       <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="1" t="n">
+      <c r="D36" s="1">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G36" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H36" s="1" t="n">
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>20</v>
+      </c>
+      <c r="H36" s="1">
         <v>0.2</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -1447,44 +1708,36 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMK24"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1619433198381"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="13.53125" style="1"/>
+    <col min="3" max="3" width="36.06640625" style="1"/>
+    <col min="4" max="4" width="11.46484375" style="1"/>
+    <col min="5" max="5" width="12.1328125" style="1"/>
+    <col min="6" max="6" width="12.19921875" style="1"/>
+    <col min="7" max="7" width="7.265625" style="1"/>
+    <col min="8" max="8" width="15.3984375" style="1"/>
+    <col min="9" max="9" width="11.46484375" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1513,61 +1766,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="0"/>
+      <c r="B2"/>
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="0"/>
+      <c r="B3"/>
       <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1577,53 +1830,53 @@
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="n">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="0"/>
+      <c r="B5"/>
       <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1" t="n">
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1633,134 +1886,134 @@
       <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1" t="n">
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="0"/>
+      <c r="B7"/>
       <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="n">
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
         <v>0.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="0"/>
+      <c r="B8"/>
       <c r="C8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1" t="n">
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1">
         <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="0"/>
+      <c r="B9"/>
       <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1" t="n">
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1">
         <v>0.2</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="0"/>
+      <c r="B10"/>
       <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1" t="n">
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1">
         <v>0.2</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -1770,26 +2023,26 @@
       <c r="C11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -1799,26 +2052,26 @@
       <c r="C12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -1828,26 +2081,26 @@
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1857,26 +2110,26 @@
       <c r="C14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1" t="n">
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
@@ -1886,26 +2139,26 @@
       <c r="C15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>4</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -1915,26 +2168,26 @@
       <c r="C16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1" t="n">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
@@ -1944,26 +2197,26 @@
       <c r="C17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1" t="n">
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -1973,26 +2226,26 @@
       <c r="C18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="n">
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -2002,7 +2255,7 @@
       <c r="C19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -2014,14 +2267,14 @@
       <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="1">
         <v>0.1</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -2031,7 +2284,7 @@
       <c r="C20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2043,14 +2296,14 @@
       <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="H20" s="1">
         <v>0.1</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -2060,26 +2313,26 @@
       <c r="C21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="n">
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
         <v>0.4</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
         <v>79</v>
       </c>
@@ -2089,26 +2342,26 @@
       <c r="C22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="n">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -2118,32 +2371,56 @@
       <c r="C23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="1">
         <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="n">
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="1">
+        <v>20</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new chest reopening concept 3 vertices running on all printers
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ACDFE7-DB0B-4C97-9B44-4E04EE24DD6E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7F6ABA-A7DE-4E40-953B-4986EFAB92BC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="92">
   <si>
     <t>Date Requested</t>
   </si>
@@ -283,6 +283,21 @@
   </si>
   <si>
     <t>Tracheal Rings od: 23.5 id: 15.5</t>
+  </si>
+  <si>
+    <t>27-06-2018</t>
+  </si>
+  <si>
+    <t>Chest Reopening Concept 3 Top Front Verticies</t>
+  </si>
+  <si>
+    <t>Chest Reopening Concept 3 Top Back Verticies</t>
+  </si>
+  <si>
+    <t>Chest Reopening Concept 3 Bot Front Verticies</t>
+  </si>
+  <si>
+    <t>Chest Reopening Concept 3 Bot Back Verticies</t>
   </si>
 </sst>
 </file>
@@ -1715,19 +1730,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK24"/>
+  <dimension ref="A1:AMK28"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.796875" style="1"/>
     <col min="2" max="2" width="13.53125" style="1"/>
-    <col min="3" max="3" width="36.06640625" style="1"/>
+    <col min="3" max="3" width="37.9296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.46484375" style="1"/>
     <col min="5" max="5" width="12.1328125" style="1"/>
     <col min="6" max="6" width="12.19921875" style="1"/>
@@ -2419,6 +2434,122 @@
         <v>11</v>
       </c>
     </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
added more pieces for the chest reopening phantom concept 3
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7F6ABA-A7DE-4E40-953B-4986EFAB92BC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F2151F-97C5-4442-AE32-886A6A1125DE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="95">
   <si>
     <t>Date Requested</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>Chest Reopening Concept 3 Bot Back Verticies</t>
+  </si>
+  <si>
+    <t>28-06-2018</t>
+  </si>
+  <si>
+    <t>Chest Reopening Concept 3 Midstops</t>
+  </si>
+  <si>
+    <t>Chest Reopening Concept 3 Left + Right Sternum</t>
   </si>
 </sst>
 </file>
@@ -1730,19 +1739,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK28"/>
+  <dimension ref="A1:AMK30"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J28" sqref="J28:K28"/>
+      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.796875" style="1"/>
     <col min="2" max="2" width="13.53125" style="1"/>
-    <col min="3" max="3" width="37.9296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.46484375" style="1"/>
     <col min="5" max="5" width="12.1328125" style="1"/>
     <col min="6" max="6" width="12.19921875" style="1"/>
@@ -2550,6 +2559,64 @@
         <v>11</v>
       </c>
     </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="1">
+        <v>4</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3</v>
+      </c>
+      <c r="G29" s="1">
+        <v>20</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>20</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
added request for 200 tracheal rings and fixed completion date for chest reopening concept 3 sternum pieces
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F2151F-97C5-4442-AE32-886A6A1125DE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAA0701-021D-468B-97F0-C8E8A1DEE0A0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="97">
   <si>
     <t>Date Requested</t>
   </si>
@@ -307,6 +307,12 @@
   </si>
   <si>
     <t>Chest Reopening Concept 3 Left + Right Sternum</t>
+  </si>
+  <si>
+    <t>29-06-2018</t>
+  </si>
+  <si>
+    <t>Polylite/PLA</t>
   </si>
 </sst>
 </file>
@@ -1739,12 +1745,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK30"/>
+  <dimension ref="A1:AMK31"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2593,7 +2599,7 @@
         <v>92</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>94</v>
@@ -2614,6 +2620,32 @@
         <v>0.4</v>
       </c>
       <c r="I30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="1">
+        <v>200</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new tab for July and pieces for the vaulted IR phantom mold
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845189E5-85FB-4323-B0D0-1DAB00DF7C01}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="May 2018" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="June 2018" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="May 2018" sheetId="1" r:id="rId1"/>
+    <sheet name="June 2018" sheetId="2" r:id="rId2"/>
+    <sheet name="July 2018" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="101">
   <si>
     <t>Date Requested</t>
   </si>
@@ -307,18 +314,28 @@
   </si>
   <si>
     <t>Polylite/PLA</t>
+  </si>
+  <si>
+    <t>02-07-2018</t>
+  </si>
+  <si>
+    <t>Vaulted IR Phantom - Body</t>
+  </si>
+  <si>
+    <t>Bridge</t>
+  </si>
+  <si>
+    <t>Vaulted IR Phantom - Ends</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="DD/MMM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -327,22 +344,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -359,7 +361,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -367,96 +369,362 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK36"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.39676113360324"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="13.53125" style="1"/>
+    <col min="3" max="3" width="36.06640625" style="1"/>
+    <col min="4" max="4" width="11.46484375" style="1"/>
+    <col min="5" max="5" width="9.3984375" style="1"/>
+    <col min="6" max="6" width="12.19921875" style="1"/>
+    <col min="7" max="7" width="7.265625" style="1"/>
+    <col min="8" max="8" width="15.3984375" style="1"/>
+    <col min="9" max="9" width="11.46484375" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -485,17 +753,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="3">
         <v>43224</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="3">
         <v>43224</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -507,24 +775,24 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1">
         <v>0.1</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="3">
         <v>43224</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="3">
         <v>43225</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -536,24 +804,24 @@
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="1">
         <v>0.1</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="3">
         <v>43224</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="3">
         <v>43225</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -565,24 +833,24 @@
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="1">
         <v>0.1</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="3">
         <v>43224</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="3">
         <v>43226</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -594,24 +862,24 @@
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="1">
         <v>0.1</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="3">
         <v>43224</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="3">
         <v>43227</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -623,24 +891,24 @@
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="1">
         <v>0.1</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="3">
         <v>43224</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="3">
         <v>43228</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -652,24 +920,24 @@
       <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="1">
         <v>0.1</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="3">
         <v>43224</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="3">
         <v>43242</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -681,15 +949,15 @@
       <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="1">
         <v>0.1</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="3">
         <v>43224</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -698,7 +966,7 @@
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -710,15 +978,15 @@
       <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H9" s="1">
         <v>0.1</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="3">
         <v>43224</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -727,7 +995,7 @@
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -739,160 +1007,160 @@
       <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="1">
         <v>0.1</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="3">
         <v>43238</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="3">
         <v>43242</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="3">
         <v>43238</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="3">
         <v>43242</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="3">
         <v>43238</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="3">
         <v>43242</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="3">
         <v>43238</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="3">
         <v>43242</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="n">
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
         <v>100</v>
       </c>
-      <c r="H14" s="1" t="n">
+      <c r="H14" s="1">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="3">
         <v>43238</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="3">
         <v>43242</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="3">
         <v>43242</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -901,27 +1169,27 @@
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1" t="n">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="3">
         <v>43242</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -930,27 +1198,27 @@
       <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1" t="n">
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="3">
         <v>43242</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -959,26 +1227,26 @@
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="n">
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -988,53 +1256,53 @@
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" s="1" t="n">
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
         <v>100</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="1">
         <v>0.2</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="0"/>
+      <c r="B20"/>
       <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="1">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="n">
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1">
         <v>0.2</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -1044,161 +1312,161 @@
       <c r="C21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="n">
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
         <v>0.2</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="0"/>
+      <c r="B22"/>
       <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="n">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="0"/>
+      <c r="B23"/>
       <c r="C23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="1">
         <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="n">
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="0"/>
+      <c r="B24"/>
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="1">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1" t="n">
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="0"/>
+      <c r="B25"/>
       <c r="C25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="1">
         <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1" t="n">
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="0"/>
+      <c r="B26"/>
       <c r="C26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="1">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1" t="n">
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1208,26 +1476,26 @@
       <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="1">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1" t="n">
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1237,26 +1505,26 @@
       <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="1">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1" t="n">
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -1266,26 +1534,26 @@
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1" t="n">
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
         <v>10</v>
       </c>
-      <c r="H29" s="1" t="n">
+      <c r="H29" s="1">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -1295,7 +1563,7 @@
       <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1307,95 +1575,95 @@
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="1" t="n">
+      <c r="H30" s="1">
         <v>0.2</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="0"/>
+      <c r="B31"/>
       <c r="C31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="D31" s="1">
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1" t="n">
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="0"/>
+      <c r="B32"/>
       <c r="C32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="1" t="n">
+      <c r="D32" s="1">
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G32" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H32" s="1" t="n">
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>20</v>
+      </c>
+      <c r="H32" s="1">
         <v>0.2</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="0"/>
+      <c r="B33"/>
       <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="1" t="n">
+      <c r="D33" s="1">
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H33" s="1" t="n">
+      <c r="F33" s="1">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1">
         <v>0.2</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -1405,26 +1673,26 @@
       <c r="C34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="1" t="n">
+      <c r="D34" s="1">
         <v>15</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G34" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H34" s="1" t="n">
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>20</v>
+      </c>
+      <c r="H34" s="1">
         <v>0.2</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
@@ -1434,26 +1702,26 @@
       <c r="C35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="1" t="n">
+      <c r="D35" s="1">
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H35" s="1" t="n">
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1">
         <v>0.2</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
@@ -1463,19 +1731,19 @@
       <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="1" t="n">
+      <c r="D36" s="1">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G36" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H36" s="1" t="n">
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>20</v>
+      </c>
+      <c r="H36" s="1">
         <v>0.2</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -1483,44 +1751,35 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMK31"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1336032388664"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="13.53125" style="1"/>
+    <col min="3" max="3" width="39.265625" style="1"/>
+    <col min="4" max="4" width="11.46484375" style="1"/>
+    <col min="5" max="5" width="12.1328125" style="1"/>
+    <col min="6" max="6" width="12.19921875" style="1"/>
+    <col min="7" max="7" width="7.265625" style="1"/>
+    <col min="8" max="8" width="15.3984375" style="1"/>
+    <col min="9" max="9" width="11.46484375" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1549,61 +1808,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="0"/>
+      <c r="B2"/>
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="0"/>
+      <c r="B3"/>
       <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1613,53 +1872,53 @@
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="n">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="0"/>
+      <c r="B5"/>
       <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1" t="n">
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1669,134 +1928,134 @@
       <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1" t="n">
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="0"/>
+      <c r="B7"/>
       <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="n">
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
         <v>0.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="0"/>
+      <c r="B8"/>
       <c r="C8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1" t="n">
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1">
         <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="0"/>
+      <c r="B9"/>
       <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1" t="n">
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1">
         <v>0.2</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="0"/>
+      <c r="B10"/>
       <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1" t="n">
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1">
         <v>0.2</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -1806,26 +2065,26 @@
       <c r="C11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -1835,26 +2094,26 @@
       <c r="C12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -1864,26 +2123,26 @@
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1893,26 +2152,26 @@
       <c r="C14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1" t="n">
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
@@ -1922,26 +2181,26 @@
       <c r="C15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>4</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -1951,26 +2210,26 @@
       <c r="C16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1" t="n">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
@@ -1980,26 +2239,26 @@
       <c r="C17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1" t="n">
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -2009,26 +2268,26 @@
       <c r="C18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="n">
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -2038,7 +2297,7 @@
       <c r="C19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -2050,14 +2309,14 @@
       <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="1">
         <v>0.1</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -2067,7 +2326,7 @@
       <c r="C20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2079,14 +2338,14 @@
       <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="H20" s="1">
         <v>0.1</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -2096,26 +2355,26 @@
       <c r="C21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="n">
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
         <v>0.4</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
         <v>79</v>
       </c>
@@ -2125,26 +2384,26 @@
       <c r="C22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="n">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -2154,26 +2413,26 @@
       <c r="C23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="1">
         <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="n">
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>85</v>
       </c>
@@ -2183,26 +2442,26 @@
       <c r="C24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="1">
         <v>20</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1" t="n">
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -2212,26 +2471,26 @@
       <c r="C25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="1">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1" t="n">
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>87</v>
       </c>
@@ -2241,26 +2500,26 @@
       <c r="C26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="1">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1" t="n">
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>87</v>
       </c>
@@ -2270,26 +2529,26 @@
       <c r="C27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="1">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1" t="n">
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>87</v>
       </c>
@@ -2299,26 +2558,26 @@
       <c r="C28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="1">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1" t="n">
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>92</v>
       </c>
@@ -2328,26 +2587,26 @@
       <c r="C29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D29" s="1">
         <v>4</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="1" t="n">
+      <c r="F29" s="1">
         <v>3</v>
       </c>
-      <c r="G29" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H29" s="1" t="n">
+      <c r="G29" s="1">
+        <v>20</v>
+      </c>
+      <c r="H29" s="1">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
@@ -2357,26 +2616,26 @@
       <c r="C30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G30" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H30" s="1" t="n">
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>20</v>
+      </c>
+      <c r="H30" s="1">
         <v>0.4</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -2386,19 +2645,19 @@
       <c r="C31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="D31" s="1">
         <v>200</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1" t="n">
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -2406,12 +2665,144 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9BC9B2C-69C2-4E23-9A4E-A1504433AF49}">
+  <dimension ref="A1:AMK22"/>
+  <sheetViews>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.06640625" style="1"/>
+    <col min="5" max="5" width="7.53125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.53125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B10"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added completion of IR mold pieces and request for new TEE track
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845189E5-85FB-4323-B0D0-1DAB00DF7C01}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98223565-F161-4EA6-AD33-4FDF1679B02C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="104">
   <si>
     <t>Date Requested</t>
   </si>
@@ -326,6 +326,15 @@
   </si>
   <si>
     <t>Vaulted IR Phantom - Ends</t>
+  </si>
+  <si>
+    <t>04-07-2018</t>
+  </si>
+  <si>
+    <t>03-07-2018</t>
+  </si>
+  <si>
+    <t>EVHP Concept 5 TEE Track Wide Bore</t>
   </si>
 </sst>
 </file>
@@ -2676,7 +2685,7 @@
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2726,7 +2735,9 @@
       <c r="A2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B2"/>
+      <c r="B2" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>98</v>
       </c>
@@ -2753,7 +2764,9 @@
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B3"/>
+      <c r="B3" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>100</v>
       </c>
@@ -2777,7 +2790,31 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="B4" s="4"/>
+      <c r="C4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B5"/>

</xml_diff>

<commit_message>
added request for experimental spine in a box
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98223565-F161-4EA6-AD33-4FDF1679B02C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12028DCE-4BF1-4CA5-9751-C67D480BC8F4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="107">
   <si>
     <t>Date Requested</t>
   </si>
@@ -335,6 +335,15 @@
   </si>
   <si>
     <t>EVHP Concept 5 TEE Track Wide Bore</t>
+  </si>
+  <si>
+    <t>04-08-2018</t>
+  </si>
+  <si>
+    <t>16-07-2018</t>
+  </si>
+  <si>
+    <t>Spine in a Box 3lvl Spine</t>
   </si>
 </sst>
 </file>
@@ -2685,7 +2694,7 @@
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2793,7 +2802,9 @@
       <c r="A4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>103</v>
       </c>
@@ -2817,7 +2828,31 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="B5"/>
+      <c r="C5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B6" s="4"/>

</xml_diff>

<commit_message>
completed 3lvl spine with ends
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -1,29 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12028DCE-4BF1-4CA5-9751-C67D480BC8F4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection lockWindows="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="May 2018" sheetId="1" r:id="rId1"/>
-    <sheet name="June 2018" sheetId="2" r:id="rId2"/>
-    <sheet name="July 2018" sheetId="3" r:id="rId3"/>
+    <sheet name="May 2018" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="June 2018" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="July 2018" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="107">
   <si>
     <t>Date Requested</t>
   </si>
@@ -319,6 +313,9 @@
     <t>02-07-2018</t>
   </si>
   <si>
+    <t>03-07-2018</t>
+  </si>
+  <si>
     <t>Vaulted IR Phantom - Body</t>
   </si>
   <si>
@@ -331,13 +328,10 @@
     <t>04-07-2018</t>
   </si>
   <si>
-    <t>03-07-2018</t>
+    <t>04-08-2018</t>
   </si>
   <si>
     <t>EVHP Concept 5 TEE Track Wide Bore</t>
-  </si>
-  <si>
-    <t>04-08-2018</t>
   </si>
   <si>
     <t>16-07-2018</t>
@@ -349,11 +343,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MMM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -362,7 +358,22 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -379,7 +390,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -387,362 +398,96 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A36" activeCellId="1" sqref="B5 A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.796875" style="1"/>
-    <col min="2" max="2" width="13.53125" style="1"/>
-    <col min="3" max="3" width="36.06640625" style="1"/>
-    <col min="4" max="4" width="11.46484375" style="1"/>
-    <col min="5" max="5" width="9.3984375" style="1"/>
-    <col min="6" max="6" width="12.19921875" style="1"/>
-    <col min="7" max="7" width="7.265625" style="1"/>
-    <col min="8" max="8" width="15.3984375" style="1"/>
-    <col min="9" max="9" width="11.46484375" style="1"/>
-    <col min="10" max="1025" width="9.06640625" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.0647773279352"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.39676113360324"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -771,17 +516,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="3">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="3" t="n">
         <v>43224</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -793,24 +538,24 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="3">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="3" t="n">
         <v>43225</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -822,24 +567,24 @@
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="3">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="3" t="n">
         <v>43225</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -851,24 +596,24 @@
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="3">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="3" t="n">
         <v>43226</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -880,24 +625,24 @@
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="3">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="3" t="n">
         <v>43227</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -909,24 +654,24 @@
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="3">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="n">
         <v>43228</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -938,24 +683,24 @@
       <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="3">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -967,15 +712,15 @@
       <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="3">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
         <v>43224</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -984,7 +729,7 @@
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -996,15 +741,15 @@
       <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="3">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
         <v>43224</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1013,7 +758,7 @@
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1025,160 +770,160 @@
       <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="3">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="F11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="3">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="F12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="3">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="F13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="3">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1">
+      <c r="F14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="3">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="F15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="3">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1187,27 +932,27 @@
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1">
+      <c r="F16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="3">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1216,27 +961,27 @@
       <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="F17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A18" s="3">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1245,26 +990,26 @@
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="F18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1274,53 +1019,53 @@
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="1">
-        <v>2</v>
-      </c>
-      <c r="G19" s="1">
+      <c r="F19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20"/>
+      <c r="B20" s="0"/>
       <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="1">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1">
+      <c r="F20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -1330,161 +1075,161 @@
       <c r="C21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1">
+      <c r="F21" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22"/>
+      <c r="B22" s="0"/>
       <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="F22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23"/>
+      <c r="B23" s="0"/>
       <c r="C23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1">
+      <c r="F23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24"/>
+      <c r="B24" s="0"/>
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1">
+      <c r="F24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25"/>
+      <c r="B25" s="0"/>
       <c r="C25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="F25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26"/>
+      <c r="B26" s="0"/>
       <c r="C26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="F26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1494,26 +1239,26 @@
       <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="1">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="F27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1523,26 +1268,26 @@
       <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="1">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1">
+      <c r="F28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -1552,26 +1297,26 @@
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1">
+      <c r="F29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -1581,7 +1326,7 @@
       <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1593,95 +1338,95 @@
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="1">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1">
+      <c r="F31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32"/>
+      <c r="B32" s="0"/>
       <c r="C32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="1">
-        <v>2</v>
-      </c>
-      <c r="G32" s="1">
-        <v>20</v>
-      </c>
-      <c r="H32" s="1">
+      <c r="F32" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H32" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="1">
-        <v>2</v>
-      </c>
-      <c r="G33" s="1">
-        <v>20</v>
-      </c>
-      <c r="H33" s="1">
+      <c r="F33" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -1691,26 +1436,26 @@
       <c r="C34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="1" t="n">
         <v>15</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="1">
-        <v>2</v>
-      </c>
-      <c r="G34" s="1">
-        <v>20</v>
-      </c>
-      <c r="H34" s="1">
+      <c r="F34" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H34" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
@@ -1720,26 +1465,26 @@
       <c r="C35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="1">
-        <v>2</v>
-      </c>
-      <c r="G35" s="1">
-        <v>20</v>
-      </c>
-      <c r="H35" s="1">
+      <c r="F35" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
@@ -1749,19 +1494,19 @@
       <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="1">
-        <v>2</v>
-      </c>
-      <c r="G36" s="1">
-        <v>20</v>
-      </c>
-      <c r="H36" s="1">
+      <c r="F36" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H36" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -1769,35 +1514,44 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="1" sqref="B5 A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.796875" style="1"/>
-    <col min="2" max="2" width="13.53125" style="1"/>
-    <col min="3" max="3" width="39.265625" style="1"/>
-    <col min="4" max="4" width="11.46484375" style="1"/>
-    <col min="5" max="5" width="12.1328125" style="1"/>
-    <col min="6" max="6" width="12.19921875" style="1"/>
-    <col min="7" max="7" width="7.265625" style="1"/>
-    <col min="8" max="8" width="15.3984375" style="1"/>
-    <col min="9" max="9" width="11.46484375" style="1"/>
-    <col min="10" max="1025" width="9.06640625" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1336032388664"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1826,61 +1580,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2"/>
+      <c r="B2" s="0"/>
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="F2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3"/>
+      <c r="B3" s="0"/>
       <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="F3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1890,53 +1644,53 @@
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="F4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" s="0"/>
       <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="F5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1946,134 +1700,134 @@
       <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="F6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7"/>
+      <c r="B7" s="0"/>
       <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="F7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" s="0"/>
       <c r="C8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="F8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9"/>
+      <c r="B9" s="0"/>
       <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="F9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" s="0"/>
       <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1">
+      <c r="F10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -2083,26 +1837,26 @@
       <c r="C11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="F11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -2112,26 +1866,26 @@
       <c r="C12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="F12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -2141,26 +1895,26 @@
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="F13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -2170,26 +1924,26 @@
       <c r="C14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1">
+      <c r="F14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
@@ -2199,26 +1953,26 @@
       <c r="C15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="F15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -2228,26 +1982,26 @@
       <c r="C16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1">
+      <c r="F16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
@@ -2257,26 +2011,26 @@
       <c r="C17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="F17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -2286,26 +2040,26 @@
       <c r="C18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="1" t="n">
         <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="F18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -2315,7 +2069,7 @@
       <c r="C19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="1" t="n">
         <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -2327,14 +2081,14 @@
       <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -2344,7 +2098,7 @@
       <c r="C20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2356,14 +2110,14 @@
       <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -2373,26 +2127,26 @@
       <c r="C21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1">
+      <c r="F21" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <v>0.4</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
         <v>79</v>
       </c>
@@ -2402,26 +2156,26 @@
       <c r="C22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="F22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -2431,26 +2185,26 @@
       <c r="C23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1">
+      <c r="F23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>85</v>
       </c>
@@ -2460,26 +2214,26 @@
       <c r="C24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="1" t="n">
         <v>20</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1">
+      <c r="F24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -2489,26 +2243,26 @@
       <c r="C25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="F25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>87</v>
       </c>
@@ -2518,26 +2272,26 @@
       <c r="C26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="F26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>87</v>
       </c>
@@ -2547,26 +2301,26 @@
       <c r="C27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="1">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="F27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>87</v>
       </c>
@@ -2576,26 +2330,26 @@
       <c r="C28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="1">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1">
+      <c r="F28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>92</v>
       </c>
@@ -2605,26 +2359,26 @@
       <c r="C29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G29" s="1">
-        <v>20</v>
-      </c>
-      <c r="H29" s="1">
+      <c r="G29" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H29" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
@@ -2634,26 +2388,26 @@
       <c r="C30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="1">
-        <v>2</v>
-      </c>
-      <c r="G30" s="1">
-        <v>20</v>
-      </c>
-      <c r="H30" s="1">
+      <c r="F30" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H30" s="1" t="n">
         <v>0.4</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -2663,19 +2417,19 @@
       <c r="C31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="1" t="n">
         <v>200</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="1">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1">
+      <c r="F31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -2683,35 +2437,44 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9BC9B2C-69C2-4E23-9A4E-A1504433AF49}">
-  <dimension ref="A1:AMK22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.06640625" style="1"/>
-    <col min="5" max="5" width="7.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="1025" width="9.06640625" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.52631578947368"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.5991902834008"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.39676113360324"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7975708502024"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.53441295546559"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2740,141 +2503,129 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="1">
+        <v>99</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="B4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="F4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1">
+        <v>100</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B10"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed name and added prints for spine box case and lid
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67F689E-A95E-4536-8AE7-F6D96AA73B08}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="May 2018" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="June 2018" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="July 2018" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="May 2018" sheetId="1" r:id="rId1"/>
+    <sheet name="June 2018" sheetId="2" r:id="rId2"/>
+    <sheet name="July 2018" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="110">
   <si>
     <t>Date Requested</t>
   </si>
@@ -338,18 +344,25 @@
   </si>
   <si>
     <t>Spine in a Box 3lvl Spine</t>
+  </si>
+  <si>
+    <t>17-07-2018</t>
+  </si>
+  <si>
+    <t>Spine Box Case</t>
+  </si>
+  <si>
+    <t>Spine Box Lid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="DD/MMM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -358,22 +371,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -390,7 +388,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -398,96 +396,362 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK36"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A36" activeCellId="1" sqref="B5 A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.39676113360324"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="13.53125" style="1"/>
+    <col min="3" max="3" width="36.06640625" style="1"/>
+    <col min="4" max="4" width="11.46484375" style="1"/>
+    <col min="5" max="5" width="9.3984375" style="1"/>
+    <col min="6" max="6" width="12.19921875" style="1"/>
+    <col min="7" max="7" width="7.265625" style="1"/>
+    <col min="8" max="8" width="15.3984375" style="1"/>
+    <col min="9" max="9" width="11.46484375" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -516,17 +780,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="3">
         <v>43224</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="3">
         <v>43224</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -538,24 +802,24 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1">
         <v>0.1</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="3">
         <v>43224</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="3">
         <v>43225</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -567,24 +831,24 @@
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="1">
         <v>0.1</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="3">
         <v>43224</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="3">
         <v>43225</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -596,24 +860,24 @@
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="1">
         <v>0.1</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="3">
         <v>43224</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="3">
         <v>43226</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -625,24 +889,24 @@
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="1">
         <v>0.1</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="3">
         <v>43224</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="3">
         <v>43227</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -654,24 +918,24 @@
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="1">
         <v>0.1</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="3">
         <v>43224</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="3">
         <v>43228</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -683,24 +947,24 @@
       <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="1">
         <v>0.1</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="3">
         <v>43224</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="3">
         <v>43242</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -712,15 +976,15 @@
       <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="1">
         <v>0.1</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="3">
         <v>43224</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -729,7 +993,7 @@
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -741,15 +1005,15 @@
       <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H9" s="1">
         <v>0.1</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="3">
         <v>43224</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -758,7 +1022,7 @@
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -770,160 +1034,160 @@
       <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="1">
         <v>0.1</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="3">
         <v>43238</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="3">
         <v>43242</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="3">
         <v>43238</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="3">
         <v>43242</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="3">
         <v>43238</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="3">
         <v>43242</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="3">
         <v>43238</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="3">
         <v>43242</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="n">
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
         <v>100</v>
       </c>
-      <c r="H14" s="1" t="n">
+      <c r="H14" s="1">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="3">
         <v>43238</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="3">
         <v>43242</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="3">
         <v>43242</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -932,27 +1196,27 @@
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1" t="n">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="3">
         <v>43242</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -961,27 +1225,27 @@
       <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1" t="n">
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="3">
         <v>43242</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -990,26 +1254,26 @@
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="n">
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1019,53 +1283,53 @@
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" s="1" t="n">
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
         <v>100</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="1">
         <v>0.2</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="0"/>
+      <c r="B20"/>
       <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="1">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="n">
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1">
         <v>0.2</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -1075,161 +1339,161 @@
       <c r="C21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="n">
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
         <v>0.2</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="0"/>
+      <c r="B22"/>
       <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="n">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="0"/>
+      <c r="B23"/>
       <c r="C23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="1">
         <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="n">
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="0"/>
+      <c r="B24"/>
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="1">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1" t="n">
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="0"/>
+      <c r="B25"/>
       <c r="C25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="1">
         <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1" t="n">
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="0"/>
+      <c r="B26"/>
       <c r="C26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="1">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1" t="n">
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1239,26 +1503,26 @@
       <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="1">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1" t="n">
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1268,26 +1532,26 @@
       <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="1">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1" t="n">
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -1297,26 +1561,26 @@
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1" t="n">
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
         <v>10</v>
       </c>
-      <c r="H29" s="1" t="n">
+      <c r="H29" s="1">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -1326,7 +1590,7 @@
       <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1338,95 +1602,95 @@
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="1" t="n">
+      <c r="H30" s="1">
         <v>0.2</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="0"/>
+      <c r="B31"/>
       <c r="C31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="D31" s="1">
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1" t="n">
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="0"/>
+      <c r="B32"/>
       <c r="C32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="1" t="n">
+      <c r="D32" s="1">
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G32" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H32" s="1" t="n">
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>20</v>
+      </c>
+      <c r="H32" s="1">
         <v>0.2</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="0"/>
+      <c r="B33"/>
       <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="1" t="n">
+      <c r="D33" s="1">
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H33" s="1" t="n">
+      <c r="F33" s="1">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1">
         <v>0.2</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -1436,26 +1700,26 @@
       <c r="C34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="1" t="n">
+      <c r="D34" s="1">
         <v>15</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G34" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H34" s="1" t="n">
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>20</v>
+      </c>
+      <c r="H34" s="1">
         <v>0.2</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
@@ -1465,26 +1729,26 @@
       <c r="C35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="1" t="n">
+      <c r="D35" s="1">
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H35" s="1" t="n">
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1">
         <v>0.2</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
@@ -1494,19 +1758,19 @@
       <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="1" t="n">
+      <c r="D36" s="1">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G36" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H36" s="1" t="n">
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>20</v>
+      </c>
+      <c r="H36" s="1">
         <v>0.2</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -1514,44 +1778,35 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMK31"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A32" activeCellId="1" sqref="B5 A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1336032388664"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="13.53125" style="1"/>
+    <col min="3" max="3" width="39.265625" style="1"/>
+    <col min="4" max="4" width="11.46484375" style="1"/>
+    <col min="5" max="5" width="12.1328125" style="1"/>
+    <col min="6" max="6" width="12.19921875" style="1"/>
+    <col min="7" max="7" width="7.265625" style="1"/>
+    <col min="8" max="8" width="15.3984375" style="1"/>
+    <col min="9" max="9" width="11.46484375" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1580,61 +1835,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="0"/>
+      <c r="B2"/>
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="0"/>
+      <c r="B3"/>
       <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1644,53 +1899,53 @@
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="n">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="0"/>
+      <c r="B5"/>
       <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1" t="n">
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1700,134 +1955,134 @@
       <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1" t="n">
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="0"/>
+      <c r="B7"/>
       <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="n">
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
         <v>0.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="0"/>
+      <c r="B8"/>
       <c r="C8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1" t="n">
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1">
         <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="0"/>
+      <c r="B9"/>
       <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1" t="n">
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1">
         <v>0.2</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="0"/>
+      <c r="B10"/>
       <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1" t="n">
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1">
         <v>0.2</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -1837,26 +2092,26 @@
       <c r="C11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -1866,26 +2121,26 @@
       <c r="C12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -1895,26 +2150,26 @@
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1924,26 +2179,26 @@
       <c r="C14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1" t="n">
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
@@ -1953,26 +2208,26 @@
       <c r="C15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>4</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -1982,26 +2237,26 @@
       <c r="C16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1" t="n">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
@@ -2011,26 +2266,26 @@
       <c r="C17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1" t="n">
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -2040,26 +2295,26 @@
       <c r="C18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="n">
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -2069,7 +2324,7 @@
       <c r="C19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -2081,14 +2336,14 @@
       <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="1">
         <v>0.1</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -2098,7 +2353,7 @@
       <c r="C20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2110,14 +2365,14 @@
       <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="H20" s="1">
         <v>0.1</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -2127,26 +2382,26 @@
       <c r="C21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="n">
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
         <v>0.4</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
         <v>79</v>
       </c>
@@ -2156,26 +2411,26 @@
       <c r="C22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="n">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -2185,26 +2440,26 @@
       <c r="C23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="1">
         <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="n">
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>85</v>
       </c>
@@ -2214,26 +2469,26 @@
       <c r="C24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="1">
         <v>20</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1" t="n">
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -2243,26 +2498,26 @@
       <c r="C25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="1">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1" t="n">
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>87</v>
       </c>
@@ -2272,26 +2527,26 @@
       <c r="C26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="1">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1" t="n">
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>87</v>
       </c>
@@ -2301,26 +2556,26 @@
       <c r="C27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="1">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1" t="n">
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>87</v>
       </c>
@@ -2330,26 +2585,26 @@
       <c r="C28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="1">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1" t="n">
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>92</v>
       </c>
@@ -2359,26 +2614,26 @@
       <c r="C29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D29" s="1">
         <v>4</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="1" t="n">
+      <c r="F29" s="1">
         <v>3</v>
       </c>
-      <c r="G29" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H29" s="1" t="n">
+      <c r="G29" s="1">
+        <v>20</v>
+      </c>
+      <c r="H29" s="1">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
@@ -2388,26 +2643,26 @@
       <c r="C30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G30" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H30" s="1" t="n">
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>20</v>
+      </c>
+      <c r="H30" s="1">
         <v>0.4</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -2417,19 +2672,19 @@
       <c r="C31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="D31" s="1">
         <v>200</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1" t="n">
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -2437,44 +2692,35 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AMK7"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9959514170041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.52631578947368"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.5991902834008"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.39676113360324"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7975708502024"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.53441295546559"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="14" style="1"/>
+    <col min="3" max="3" width="39.265625" style="1"/>
+    <col min="4" max="4" width="9.06640625" style="1"/>
+    <col min="5" max="5" width="7.53125" style="1"/>
+    <col min="6" max="6" width="12.59765625" style="1"/>
+    <col min="7" max="7" width="7.3984375" style="1"/>
+    <col min="8" max="8" width="15.796875" style="1"/>
+    <col min="9" max="9" width="9.53125" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2503,7 +2749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>97</v>
       </c>
@@ -2513,26 +2759,26 @@
       <c r="C2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -2542,26 +2788,26 @@
       <c r="C3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
@@ -2571,26 +2817,26 @@
       <c r="C4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="n">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>105</v>
       </c>
@@ -2600,32 +2846,79 @@
       <c r="C5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1" t="n">
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added requests for full set FOCUS hearts 100 scale
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67F689E-A95E-4536-8AE7-F6D96AA73B08}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695C4495-27B0-4DF5-8DEE-4243D2180D05}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="113">
   <si>
     <t>Date Requested</t>
   </si>
@@ -353,6 +353,15 @@
   </si>
   <si>
     <t>Spine Box Lid</t>
+  </si>
+  <si>
+    <t>FOCUS a4c 100 Scale</t>
+  </si>
+  <si>
+    <t>FOCUS lax 100 Scale</t>
+  </si>
+  <si>
+    <t>FOCUS sax 100 Scale</t>
   </si>
 </sst>
 </file>
@@ -2699,11 +2708,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK7"/>
+  <dimension ref="A1:AMK10"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2917,6 +2926,84 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
completed the spine box lid print
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695C4495-27B0-4DF5-8DEE-4243D2180D05}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820F7CA9-A77D-41C8-A7CC-BF793BD3E639}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="113">
   <si>
     <t>Date Requested</t>
   </si>
@@ -2712,7 +2712,7 @@
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2904,6 +2904,9 @@
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>109</v>
       </c>

</xml_diff>

<commit_message>
added the 3-lvl lumbar spine component for spine box
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -1,29 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7E6A33-05D0-40F5-B3E0-8A38E8AEED8E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection lockWindows="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="May 2018" sheetId="1" r:id="rId1"/>
-    <sheet name="June 2018" sheetId="2" r:id="rId2"/>
-    <sheet name="July 2018" sheetId="3" r:id="rId3"/>
+    <sheet name="May 2018" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="June 2018" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="July 2018" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="117">
   <si>
     <t>Date Requested</t>
   </si>
@@ -361,26 +355,31 @@
     <t>FOCUS lax 100 Scale</t>
   </si>
   <si>
+    <t>23-07-2018</t>
+  </si>
+  <si>
     <t>FOCUS sax 100 Scale</t>
   </si>
   <si>
-    <t>23-07-2018</t>
-  </si>
-  <si>
     <t>Spine Box Concept 2 Casting Case</t>
   </si>
   <si>
     <t>PCTPE</t>
+  </si>
+  <si>
+    <t>Spine Box 3-lvl Lumbar Spine Open Back</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MMM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -389,7 +388,22 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -406,7 +420,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -414,362 +428,96 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" activeCellId="1" sqref="B5 A36"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.796875" style="1"/>
-    <col min="2" max="2" width="13.53125" style="1"/>
-    <col min="3" max="3" width="36.06640625" style="1"/>
-    <col min="4" max="4" width="11.46484375" style="1"/>
-    <col min="5" max="5" width="9.3984375" style="1"/>
-    <col min="6" max="6" width="12.19921875" style="1"/>
-    <col min="7" max="7" width="7.265625" style="1"/>
-    <col min="8" max="8" width="15.3984375" style="1"/>
-    <col min="9" max="9" width="11.46484375" style="1"/>
-    <col min="10" max="1025" width="9.06640625" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.0647773279352"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.39676113360324"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -798,17 +546,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="3">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="3" t="n">
         <v>43224</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -820,24 +568,24 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="3">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="3" t="n">
         <v>43225</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -849,24 +597,24 @@
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="3">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="3" t="n">
         <v>43225</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -878,24 +626,24 @@
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="3">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="3" t="n">
         <v>43226</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -907,24 +655,24 @@
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="3">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="3" t="n">
         <v>43227</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -936,24 +684,24 @@
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="3">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="n">
         <v>43228</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -965,24 +713,24 @@
       <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="3">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -994,15 +742,15 @@
       <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="3">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
         <v>43224</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1011,7 +759,7 @@
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -1023,15 +771,15 @@
       <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="3">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
         <v>43224</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1040,7 +788,7 @@
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1052,160 +800,160 @@
       <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="3">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="F11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="3">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="F12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="3">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="F13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="3">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1">
+      <c r="F14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="3">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="F15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="3">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1214,27 +962,27 @@
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1">
+      <c r="F16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="3">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1243,27 +991,27 @@
       <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="F17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A18" s="3">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1272,26 +1020,26 @@
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="F18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1301,53 +1049,53 @@
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="1">
-        <v>2</v>
-      </c>
-      <c r="G19" s="1">
+      <c r="F19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20"/>
+      <c r="B20" s="0"/>
       <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="1">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1">
+      <c r="F20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -1357,161 +1105,161 @@
       <c r="C21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1">
+      <c r="F21" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22"/>
+      <c r="B22" s="0"/>
       <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="F22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23"/>
+      <c r="B23" s="0"/>
       <c r="C23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1">
+      <c r="F23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24"/>
+      <c r="B24" s="0"/>
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1">
+      <c r="F24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25"/>
+      <c r="B25" s="0"/>
       <c r="C25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="F25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26"/>
+      <c r="B26" s="0"/>
       <c r="C26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="F26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1521,26 +1269,26 @@
       <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="1">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="F27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1550,26 +1298,26 @@
       <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="1">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1">
+      <c r="F28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -1579,26 +1327,26 @@
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1">
+      <c r="F29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -1608,7 +1356,7 @@
       <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1620,95 +1368,95 @@
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="1">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1">
+      <c r="F31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32"/>
+      <c r="B32" s="0"/>
       <c r="C32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="1">
-        <v>2</v>
-      </c>
-      <c r="G32" s="1">
-        <v>20</v>
-      </c>
-      <c r="H32" s="1">
+      <c r="F32" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H32" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="1">
-        <v>2</v>
-      </c>
-      <c r="G33" s="1">
-        <v>20</v>
-      </c>
-      <c r="H33" s="1">
+      <c r="F33" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -1718,26 +1466,26 @@
       <c r="C34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="1" t="n">
         <v>15</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="1">
-        <v>2</v>
-      </c>
-      <c r="G34" s="1">
-        <v>20</v>
-      </c>
-      <c r="H34" s="1">
+      <c r="F34" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H34" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
@@ -1747,26 +1495,26 @@
       <c r="C35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="1">
-        <v>2</v>
-      </c>
-      <c r="G35" s="1">
-        <v>20</v>
-      </c>
-      <c r="H35" s="1">
+      <c r="F35" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
@@ -1776,19 +1524,19 @@
       <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="1">
-        <v>2</v>
-      </c>
-      <c r="G36" s="1">
-        <v>20</v>
-      </c>
-      <c r="H36" s="1">
+      <c r="F36" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H36" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -1796,35 +1544,44 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="1" sqref="B5 A32"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.796875" style="1"/>
-    <col min="2" max="2" width="13.53125" style="1"/>
-    <col min="3" max="3" width="39.265625" style="1"/>
-    <col min="4" max="4" width="11.46484375" style="1"/>
-    <col min="5" max="5" width="12.1328125" style="1"/>
-    <col min="6" max="6" width="12.19921875" style="1"/>
-    <col min="7" max="7" width="7.265625" style="1"/>
-    <col min="8" max="8" width="15.3984375" style="1"/>
-    <col min="9" max="9" width="11.46484375" style="1"/>
-    <col min="10" max="1025" width="9.06640625" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1336032388664"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1853,61 +1610,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2"/>
+      <c r="B2" s="0"/>
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="F2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3"/>
+      <c r="B3" s="0"/>
       <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="F3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1917,53 +1674,53 @@
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="F4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" s="0"/>
       <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="F5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1973,134 +1730,134 @@
       <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="F6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7"/>
+      <c r="B7" s="0"/>
       <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="F7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" s="0"/>
       <c r="C8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="F8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9"/>
+      <c r="B9" s="0"/>
       <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="F9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" s="0"/>
       <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1">
+      <c r="F10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -2110,26 +1867,26 @@
       <c r="C11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="F11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -2139,26 +1896,26 @@
       <c r="C12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="F12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -2168,26 +1925,26 @@
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="F13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -2197,26 +1954,26 @@
       <c r="C14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1">
+      <c r="F14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
@@ -2226,26 +1983,26 @@
       <c r="C15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="F15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -2255,26 +2012,26 @@
       <c r="C16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1">
+      <c r="F16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
@@ -2284,26 +2041,26 @@
       <c r="C17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="F17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -2313,26 +2070,26 @@
       <c r="C18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="1" t="n">
         <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="F18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -2342,7 +2099,7 @@
       <c r="C19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="1" t="n">
         <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -2354,14 +2111,14 @@
       <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -2371,7 +2128,7 @@
       <c r="C20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2383,14 +2140,14 @@
       <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -2400,26 +2157,26 @@
       <c r="C21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1">
+      <c r="F21" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <v>0.4</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
         <v>79</v>
       </c>
@@ -2429,26 +2186,26 @@
       <c r="C22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="F22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -2458,26 +2215,26 @@
       <c r="C23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1">
+      <c r="F23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>85</v>
       </c>
@@ -2487,26 +2244,26 @@
       <c r="C24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="1" t="n">
         <v>20</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1">
+      <c r="F24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -2516,26 +2273,26 @@
       <c r="C25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="F25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>87</v>
       </c>
@@ -2545,26 +2302,26 @@
       <c r="C26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="F26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>87</v>
       </c>
@@ -2574,26 +2331,26 @@
       <c r="C27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="1">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="F27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>87</v>
       </c>
@@ -2603,26 +2360,26 @@
       <c r="C28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="1">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1">
+      <c r="F28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>92</v>
       </c>
@@ -2632,26 +2389,26 @@
       <c r="C29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G29" s="1">
-        <v>20</v>
-      </c>
-      <c r="H29" s="1">
+      <c r="G29" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H29" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
@@ -2661,26 +2418,26 @@
       <c r="C30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="1">
-        <v>2</v>
-      </c>
-      <c r="G30" s="1">
-        <v>20</v>
-      </c>
-      <c r="H30" s="1">
+      <c r="F30" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H30" s="1" t="n">
         <v>0.4</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -2690,19 +2447,19 @@
       <c r="C31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="1" t="n">
         <v>200</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="1">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1">
+      <c r="F31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -2710,35 +2467,44 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.796875" style="1"/>
-    <col min="2" max="2" width="14" style="1"/>
-    <col min="3" max="3" width="39.265625" style="1"/>
-    <col min="4" max="4" width="9.06640625" style="1"/>
-    <col min="5" max="5" width="7.53125" style="1"/>
-    <col min="6" max="6" width="12.59765625" style="1"/>
-    <col min="7" max="7" width="7.3984375" style="1"/>
-    <col min="8" max="8" width="15.796875" style="1"/>
-    <col min="9" max="9" width="9.53125" style="1"/>
-    <col min="10" max="1025" width="9.06640625" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.52631578947368"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.5991902834008"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.39676113360324"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7975708502024"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.53441295546559"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2767,7 +2533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>97</v>
       </c>
@@ -2777,26 +2543,26 @@
       <c r="C2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="F2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -2806,26 +2572,26 @@
       <c r="C3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="F3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
@@ -2835,26 +2601,26 @@
       <c r="C4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="F4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>105</v>
       </c>
@@ -2864,52 +2630,53 @@
       <c r="C5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="1">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="F5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="B6" s="0"/>
       <c r="C6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="F6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -2919,134 +2686,167 @@
       <c r="C7" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="F7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="B8" s="0"/>
       <c r="C8" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="F8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="B9" s="0"/>
       <c r="C9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="F9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="G11" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated FOCUS SAX completion and added new Spine Box Casting Case print
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820F7CA9-A77D-41C8-A7CC-BF793BD3E639}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7E6A33-05D0-40F5-B3E0-8A38E8AEED8E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="116">
   <si>
     <t>Date Requested</t>
   </si>
@@ -362,6 +362,15 @@
   </si>
   <si>
     <t>FOCUS sax 100 Scale</t>
+  </si>
+  <si>
+    <t>23-07-2018</t>
+  </si>
+  <si>
+    <t>Spine Box Concept 2 Casting Case</t>
+  </si>
+  <si>
+    <t>PCTPE</t>
   </si>
 </sst>
 </file>
@@ -2708,11 +2717,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK10"/>
+  <dimension ref="A1:AMK11"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2985,6 +2994,9 @@
       <c r="A10" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>112</v>
       </c>
@@ -3004,6 +3016,32 @@
         <v>0.2</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added more parts for spine box concept 2
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1D667F-449B-4526-9614-DA955F2A5D89}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="May 2018" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="June 2018" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="July 2018" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="May 2018" sheetId="1" r:id="rId1"/>
+    <sheet name="June 2018" sheetId="2" r:id="rId2"/>
+    <sheet name="July 2018" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="119">
   <si>
     <t>Date Requested</t>
   </si>
@@ -368,18 +374,22 @@
   </si>
   <si>
     <t>Spine Box 3-lvl Lumbar Spine Open Back</t>
+  </si>
+  <si>
+    <t>Spine Box Concept 2 Casting Lid</t>
+  </si>
+  <si>
+    <t>Spine Box Concept 2 Casting Body</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="DD/MMM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -388,22 +398,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -420,7 +415,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -428,96 +423,362 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK36"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.39676113360324"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="13.53125" style="1"/>
+    <col min="3" max="3" width="36.06640625" style="1"/>
+    <col min="4" max="4" width="11.46484375" style="1"/>
+    <col min="5" max="5" width="9.3984375" style="1"/>
+    <col min="6" max="6" width="12.19921875" style="1"/>
+    <col min="7" max="7" width="7.265625" style="1"/>
+    <col min="8" max="8" width="15.3984375" style="1"/>
+    <col min="9" max="9" width="11.46484375" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -546,17 +807,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="3">
         <v>43224</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="3">
         <v>43224</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -568,24 +829,24 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1">
         <v>0.1</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="3">
         <v>43224</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="3">
         <v>43225</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -597,24 +858,24 @@
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="1">
         <v>0.1</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="3">
         <v>43224</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="3">
         <v>43225</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -626,24 +887,24 @@
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="1">
         <v>0.1</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="3">
         <v>43224</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="3">
         <v>43226</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -655,24 +916,24 @@
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="1">
         <v>0.1</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="3">
         <v>43224</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="3">
         <v>43227</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -684,24 +945,24 @@
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="1">
         <v>0.1</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="3">
         <v>43224</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="3">
         <v>43228</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -713,24 +974,24 @@
       <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="1">
         <v>0.1</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="3">
         <v>43224</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="3">
         <v>43242</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -742,15 +1003,15 @@
       <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="1">
         <v>0.1</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="3">
         <v>43224</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -759,7 +1020,7 @@
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -771,15 +1032,15 @@
       <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H9" s="1">
         <v>0.1</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="3">
         <v>43224</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -788,7 +1049,7 @@
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -800,160 +1061,160 @@
       <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="1">
         <v>0.1</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="3">
         <v>43238</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="3">
         <v>43242</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="3">
         <v>43238</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="3">
         <v>43242</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="3">
         <v>43238</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="3">
         <v>43242</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="3">
         <v>43238</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="3">
         <v>43242</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="n">
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
         <v>100</v>
       </c>
-      <c r="H14" s="1" t="n">
+      <c r="H14" s="1">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="3">
         <v>43238</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="3">
         <v>43242</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="3">
         <v>43242</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -962,27 +1223,27 @@
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1" t="n">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="3">
         <v>43242</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -991,27 +1252,27 @@
       <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1" t="n">
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="3">
         <v>43242</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1020,26 +1281,26 @@
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="n">
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1049,53 +1310,53 @@
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" s="1" t="n">
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
         <v>100</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="1">
         <v>0.2</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="0"/>
+      <c r="B20"/>
       <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="1">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="n">
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1">
         <v>0.2</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -1105,161 +1366,161 @@
       <c r="C21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="n">
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
         <v>0.2</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="0"/>
+      <c r="B22"/>
       <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="n">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="0"/>
+      <c r="B23"/>
       <c r="C23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="1">
         <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="n">
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="0"/>
+      <c r="B24"/>
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="1">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1" t="n">
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="0"/>
+      <c r="B25"/>
       <c r="C25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="1">
         <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1" t="n">
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="0"/>
+      <c r="B26"/>
       <c r="C26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="1">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1" t="n">
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1269,26 +1530,26 @@
       <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="1">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1" t="n">
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1298,26 +1559,26 @@
       <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="1">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1" t="n">
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -1327,26 +1588,26 @@
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1" t="n">
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
         <v>10</v>
       </c>
-      <c r="H29" s="1" t="n">
+      <c r="H29" s="1">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -1356,7 +1617,7 @@
       <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1368,95 +1629,95 @@
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="1" t="n">
+      <c r="H30" s="1">
         <v>0.2</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="0"/>
+      <c r="B31"/>
       <c r="C31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="D31" s="1">
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1" t="n">
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="0"/>
+      <c r="B32"/>
       <c r="C32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="1" t="n">
+      <c r="D32" s="1">
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G32" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H32" s="1" t="n">
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>20</v>
+      </c>
+      <c r="H32" s="1">
         <v>0.2</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="0"/>
+      <c r="B33"/>
       <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="1" t="n">
+      <c r="D33" s="1">
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H33" s="1" t="n">
+      <c r="F33" s="1">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1">
         <v>0.2</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -1466,26 +1727,26 @@
       <c r="C34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="1" t="n">
+      <c r="D34" s="1">
         <v>15</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G34" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H34" s="1" t="n">
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>20</v>
+      </c>
+      <c r="H34" s="1">
         <v>0.2</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
@@ -1495,26 +1756,26 @@
       <c r="C35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="1" t="n">
+      <c r="D35" s="1">
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H35" s="1" t="n">
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1">
         <v>0.2</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
@@ -1524,19 +1785,19 @@
       <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="1" t="n">
+      <c r="D36" s="1">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G36" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H36" s="1" t="n">
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>20</v>
+      </c>
+      <c r="H36" s="1">
         <v>0.2</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -1544,44 +1805,35 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMK31"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1336032388664"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="13.53125" style="1"/>
+    <col min="3" max="3" width="39.265625" style="1"/>
+    <col min="4" max="4" width="11.46484375" style="1"/>
+    <col min="5" max="5" width="12.1328125" style="1"/>
+    <col min="6" max="6" width="12.19921875" style="1"/>
+    <col min="7" max="7" width="7.265625" style="1"/>
+    <col min="8" max="8" width="15.3984375" style="1"/>
+    <col min="9" max="9" width="11.46484375" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1610,61 +1862,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="0"/>
+      <c r="B2"/>
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="0"/>
+      <c r="B3"/>
       <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1674,53 +1926,53 @@
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="n">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="0"/>
+      <c r="B5"/>
       <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1" t="n">
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1730,134 +1982,134 @@
       <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1" t="n">
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="0"/>
+      <c r="B7"/>
       <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="n">
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
         <v>0.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="0"/>
+      <c r="B8"/>
       <c r="C8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1" t="n">
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1">
         <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="0"/>
+      <c r="B9"/>
       <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1" t="n">
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1">
         <v>0.2</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="0"/>
+      <c r="B10"/>
       <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1" t="n">
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1">
         <v>0.2</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -1867,26 +2119,26 @@
       <c r="C11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -1896,26 +2148,26 @@
       <c r="C12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -1925,26 +2177,26 @@
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1954,26 +2206,26 @@
       <c r="C14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1" t="n">
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
@@ -1983,26 +2235,26 @@
       <c r="C15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>4</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -2012,26 +2264,26 @@
       <c r="C16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1" t="n">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
@@ -2041,26 +2293,26 @@
       <c r="C17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1" t="n">
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -2070,26 +2322,26 @@
       <c r="C18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="n">
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -2099,7 +2351,7 @@
       <c r="C19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -2111,14 +2363,14 @@
       <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="1">
         <v>0.1</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -2128,7 +2380,7 @@
       <c r="C20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2140,14 +2392,14 @@
       <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="H20" s="1">
         <v>0.1</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -2157,26 +2409,26 @@
       <c r="C21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="n">
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
         <v>0.4</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
         <v>79</v>
       </c>
@@ -2186,26 +2438,26 @@
       <c r="C22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="n">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -2215,26 +2467,26 @@
       <c r="C23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="1">
         <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="n">
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>85</v>
       </c>
@@ -2244,26 +2496,26 @@
       <c r="C24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="1">
         <v>20</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1" t="n">
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -2273,26 +2525,26 @@
       <c r="C25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="1">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1" t="n">
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>87</v>
       </c>
@@ -2302,26 +2554,26 @@
       <c r="C26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="1">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1" t="n">
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>87</v>
       </c>
@@ -2331,26 +2583,26 @@
       <c r="C27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="1">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1" t="n">
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>87</v>
       </c>
@@ -2360,26 +2612,26 @@
       <c r="C28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="1">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1" t="n">
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>92</v>
       </c>
@@ -2389,26 +2641,26 @@
       <c r="C29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D29" s="1">
         <v>4</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="1" t="n">
+      <c r="F29" s="1">
         <v>3</v>
       </c>
-      <c r="G29" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H29" s="1" t="n">
+      <c r="G29" s="1">
+        <v>20</v>
+      </c>
+      <c r="H29" s="1">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
@@ -2418,26 +2670,26 @@
       <c r="C30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G30" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H30" s="1" t="n">
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>20</v>
+      </c>
+      <c r="H30" s="1">
         <v>0.4</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -2447,19 +2699,19 @@
       <c r="C31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="D31" s="1">
         <v>200</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1" t="n">
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -2467,44 +2719,36 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AMK14"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9959514170041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.52631578947368"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.5991902834008"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.39676113360324"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7975708502024"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.53441295546559"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="14" style="1"/>
+    <col min="3" max="3" width="39.265625" style="1"/>
+    <col min="4" max="4" width="9.06640625" style="1"/>
+    <col min="5" max="5" width="7.53125" style="1"/>
+    <col min="6" max="6" width="12.59765625" style="1"/>
+    <col min="7" max="7" width="7.3984375" style="1"/>
+    <col min="8" max="8" width="15.796875" style="1"/>
+    <col min="9" max="9" width="9.53125" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2533,7 +2777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>97</v>
       </c>
@@ -2543,26 +2787,26 @@
       <c r="C2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -2572,26 +2816,26 @@
       <c r="C3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
@@ -2601,26 +2845,26 @@
       <c r="C4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="n">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>105</v>
       </c>
@@ -2630,53 +2874,53 @@
       <c r="C5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1" t="n">
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="0"/>
+      <c r="B6"/>
       <c r="C6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1" t="n">
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -2686,80 +2930,80 @@
       <c r="C7" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="n">
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
         <v>0.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="0"/>
+      <c r="B8"/>
       <c r="C8" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1" t="n">
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1">
         <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="0"/>
+      <c r="B9"/>
       <c r="C9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1" t="n">
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1">
         <v>0.2</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>107</v>
       </c>
@@ -2769,84 +3013,137 @@
       <c r="C10" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1" t="n">
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1">
         <v>0.2</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="F11" s="1">
         <v>4</v>
       </c>
-      <c r="G11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="1">
         <v>3</v>
       </c>
-      <c r="G12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed several prints for FOCUS heart order and spine box components
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1D667F-449B-4526-9614-DA955F2A5D89}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFEE3F4-67D2-4E6E-BAB3-8C3C0FEA73CA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="120">
   <si>
     <t>Date Requested</t>
   </si>
@@ -380,6 +380,9 @@
   </si>
   <si>
     <t>Spine Box Concept 2 Casting Body</t>
+  </si>
+  <si>
+    <t>24-07-2018</t>
   </si>
 </sst>
 </file>
@@ -2731,7 +2734,7 @@
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2953,7 +2956,9 @@
       <c r="A8" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>110</v>
       </c>
@@ -3094,6 +3099,9 @@
       <c r="A13" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>117</v>
       </c>
@@ -3119,6 +3127,9 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>112</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>118</v>

</xml_diff>

<commit_message>
added equipment tray prints
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFEE3F4-67D2-4E6E-BAB3-8C3C0FEA73CA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDFFC6C-1431-4A96-9E3B-19D429AEA3C6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="123">
   <si>
     <t>Date Requested</t>
   </si>
@@ -383,6 +383,15 @@
   </si>
   <si>
     <t>24-07-2018</t>
+  </si>
+  <si>
+    <t>25-07-2018</t>
+  </si>
+  <si>
+    <t>Equipment Tray Positive</t>
+  </si>
+  <si>
+    <t>Equipment Tray Clip</t>
   </si>
 </sst>
 </file>
@@ -2729,12 +2738,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK14"/>
+  <dimension ref="A1:AMK16"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3153,6 +3162,61 @@
         <v>11</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
added equipment tray holders 1 + 2 and updated completed prints
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDFFC6C-1431-4A96-9E3B-19D429AEA3C6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8146B6-59D6-4753-BE10-BEBD1A2ADA6D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="126">
   <si>
     <t>Date Requested</t>
   </si>
@@ -392,6 +392,15 @@
   </si>
   <si>
     <t>Equipment Tray Clip</t>
+  </si>
+  <si>
+    <t>26-07-2018</t>
+  </si>
+  <si>
+    <t>Equipment Tray Holder 1</t>
+  </si>
+  <si>
+    <t>Equipment Tray Holder 2</t>
   </si>
 </sst>
 </file>
@@ -2738,12 +2747,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK16"/>
+  <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2909,7 +2918,9 @@
       <c r="A6" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B6"/>
+      <c r="B6" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>108</v>
       </c>
@@ -2994,7 +3005,9 @@
       <c r="A9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B9"/>
+      <c r="B9" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>111</v>
       </c>
@@ -3195,6 +3208,9 @@
       <c r="A16" s="1" t="s">
         <v>120</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>122</v>
       </c>
@@ -3214,6 +3230,58 @@
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added reprint for FOCUS sax mid
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8146B6-59D6-4753-BE10-BEBD1A2ADA6D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D91B09-D637-4BC8-B159-CDA7CFCECE91}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="127">
   <si>
     <t>Date Requested</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>Equipment Tray Holder 2</t>
+  </si>
+  <si>
+    <t>FOCUS sax 100 Scale mid</t>
   </si>
 </sst>
 </file>
@@ -2747,12 +2750,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK18"/>
+  <dimension ref="A1:AMK19"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3285,6 +3288,35 @@
         <v>11</v>
       </c>
     </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>20</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
added first parametric Ao: stj 20, cusp to cusp 35, lvot 30
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D91B09-D637-4BC8-B159-CDA7CFCECE91}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDDDB82-6F34-4671-B918-BE835E241B64}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="128">
   <si>
     <t>Date Requested</t>
   </si>
@@ -404,6 +404,9 @@
   </si>
   <si>
     <t>FOCUS sax 100 Scale mid</t>
+  </si>
+  <si>
+    <t>parametric_ao_NA</t>
   </si>
 </sst>
 </file>
@@ -2750,12 +2753,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK19"/>
+  <dimension ref="A1:AMK20"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3317,6 +3320,35 @@
         <v>11</v>
       </c>
     </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
added measurements for parametric ao na which i think i gave the wrong dimensions to with the last commit
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDDDB82-6F34-4671-B918-BE835E241B64}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5340D3B0-E204-441D-945E-27D1660BDF86}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="129">
   <si>
     <t>Date Requested</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t>parametric_ao_NA</t>
+  </si>
+  <si>
+    <t>stj: 25 cusp: 35 lvot: 30</t>
   </si>
 </sst>
 </file>
@@ -2758,7 +2761,7 @@
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2771,7 +2774,7 @@
     <col min="6" max="6" width="12.59765625" style="1"/>
     <col min="7" max="7" width="7.3984375" style="1"/>
     <col min="8" max="8" width="15.796875" style="1"/>
-    <col min="9" max="9" width="9.53125" style="1"/>
+    <col min="9" max="9" width="19.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
@@ -3346,7 +3349,7 @@
         <v>0.2</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>11</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed equipment tray holders 1  + 2
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5340D3B0-E204-441D-945E-27D1660BDF86}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0964CDC-76EA-4A1B-8AF4-E0101E7B081E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="130">
   <si>
     <t>Date Requested</t>
   </si>
@@ -410,6 +410,9 @@
   </si>
   <si>
     <t>stj: 25 cusp: 35 lvot: 30</t>
+  </si>
+  <si>
+    <t>27-07-2018</t>
   </si>
 </sst>
 </file>
@@ -2761,7 +2764,7 @@
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3246,6 +3249,9 @@
       <c r="A17" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>124</v>
       </c>
@@ -3271,6 +3277,9 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>123</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
added request for a lot more modular blood pool pieces
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0964CDC-76EA-4A1B-8AF4-E0101E7B081E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C355FE-195A-485E-B2B3-5F805483A303}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -18,12 +18,12 @@
     <sheet name="June 2018" sheetId="2" r:id="rId2"/>
     <sheet name="July 2018" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="137">
   <si>
     <t>Date Requested</t>
   </si>
@@ -413,6 +413,27 @@
   </si>
   <si>
     <t>27-07-2018</t>
+  </si>
+  <si>
+    <t>30-07-2018</t>
+  </si>
+  <si>
+    <t>Modular heart - Ao</t>
+  </si>
+  <si>
+    <t>Modular heart - LA</t>
+  </si>
+  <si>
+    <t>Modular heart - LV</t>
+  </si>
+  <si>
+    <t>Modular heart - RV</t>
+  </si>
+  <si>
+    <t>Modular heart - RA</t>
+  </si>
+  <si>
+    <t>Modular heart - Pa</t>
   </si>
 </sst>
 </file>
@@ -2759,12 +2780,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK20"/>
+  <dimension ref="A1:AMK26"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3361,6 +3382,144 @@
         <v>128</v>
       </c>
     </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="1">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="1">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="1">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="1">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D25" s="1">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="1">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
added request for more heart base models
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C355FE-195A-485E-B2B3-5F805483A303}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C935E0-834F-4085-9EEA-DBD8708B1294}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="138">
   <si>
     <t>Date Requested</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t>Modular heart - Pa</t>
+  </si>
+  <si>
+    <t>Heart Base</t>
   </si>
 </sst>
 </file>
@@ -2780,12 +2783,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK26"/>
+  <dimension ref="A1:AMK27"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3520,6 +3523,29 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="1">
+        <v>10</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
added new sheet for august
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C935E0-834F-4085-9EEA-DBD8708B1294}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection lockWindows="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="May 2018" sheetId="1" r:id="rId1"/>
-    <sheet name="June 2018" sheetId="2" r:id="rId2"/>
-    <sheet name="July 2018" sheetId="3" r:id="rId3"/>
+    <sheet name="May 2018" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="June 2018" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="July 2018" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="August 2018" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="139">
   <si>
     <t>Date Requested</t>
   </si>
@@ -349,6 +344,9 @@
     <t>17-07-2018</t>
   </si>
   <si>
+    <t>24-07-2018</t>
+  </si>
+  <si>
     <t>Spine Box Case</t>
   </si>
   <si>
@@ -358,6 +356,9 @@
     <t>FOCUS a4c 100 Scale</t>
   </si>
   <si>
+    <t>26-07-2018</t>
+  </si>
+  <si>
     <t>FOCUS lax 100 Scale</t>
   </si>
   <si>
@@ -382,9 +383,6 @@
     <t>Spine Box Concept 2 Casting Body</t>
   </si>
   <si>
-    <t>24-07-2018</t>
-  </si>
-  <si>
     <t>25-07-2018</t>
   </si>
   <si>
@@ -394,7 +392,7 @@
     <t>Equipment Tray Clip</t>
   </si>
   <si>
-    <t>26-07-2018</t>
+    <t>27-07-2018</t>
   </si>
   <si>
     <t>Equipment Tray Holder 1</t>
@@ -412,9 +410,6 @@
     <t>stj: 25 cusp: 35 lvot: 30</t>
   </si>
   <si>
-    <t>27-07-2018</t>
-  </si>
-  <si>
     <t>30-07-2018</t>
   </si>
   <si>
@@ -437,16 +432,21 @@
   </si>
   <si>
     <t>Heart Base</t>
+  </si>
+  <si>
+    <t>01-08-2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MMM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -455,7 +455,22 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -472,7 +487,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -480,362 +495,96 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.796875" style="1"/>
-    <col min="2" max="2" width="13.53125" style="1"/>
-    <col min="3" max="3" width="36.06640625" style="1"/>
-    <col min="4" max="4" width="11.46484375" style="1"/>
-    <col min="5" max="5" width="9.3984375" style="1"/>
-    <col min="6" max="6" width="12.19921875" style="1"/>
-    <col min="7" max="7" width="7.265625" style="1"/>
-    <col min="8" max="8" width="15.3984375" style="1"/>
-    <col min="9" max="9" width="11.46484375" style="1"/>
-    <col min="10" max="1025" width="9.06640625" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.0647773279352"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.39676113360324"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -864,17 +613,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="3">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="3" t="n">
         <v>43224</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -886,24 +635,24 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="3">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="3" t="n">
         <v>43225</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -915,24 +664,24 @@
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="3">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="3" t="n">
         <v>43225</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -944,24 +693,24 @@
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="3">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="3" t="n">
         <v>43226</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -973,24 +722,24 @@
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="3">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="3" t="n">
         <v>43227</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1002,24 +751,24 @@
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="3">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="n">
         <v>43228</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1031,24 +780,24 @@
       <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="3">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
         <v>43224</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1060,15 +809,15 @@
       <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="3">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
         <v>43224</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1077,7 +826,7 @@
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -1089,15 +838,15 @@
       <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="3">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
         <v>43224</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1106,7 +855,7 @@
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1118,160 +867,160 @@
       <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="3">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="F11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="3">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="F12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="3">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="F13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="3">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1">
+      <c r="F14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="3">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="n">
         <v>43238</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="F15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="3">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1280,27 +1029,27 @@
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1">
+      <c r="F16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="3">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1309,27 +1058,27 @@
       <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="F17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A18" s="3">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="n">
         <v>43242</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1338,26 +1087,26 @@
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="F18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1367,53 +1116,53 @@
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="1">
-        <v>2</v>
-      </c>
-      <c r="G19" s="1">
+      <c r="F19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20"/>
+      <c r="B20" s="0"/>
       <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="1">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1">
+      <c r="F20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -1423,161 +1172,161 @@
       <c r="C21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1">
+      <c r="F21" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22"/>
+      <c r="B22" s="0"/>
       <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="F22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23"/>
+      <c r="B23" s="0"/>
       <c r="C23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1">
+      <c r="F23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24"/>
+      <c r="B24" s="0"/>
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1">
+      <c r="F24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25"/>
+      <c r="B25" s="0"/>
       <c r="C25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="F25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26"/>
+      <c r="B26" s="0"/>
       <c r="C26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="F26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1587,26 +1336,26 @@
       <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="1">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="F27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1616,26 +1365,26 @@
       <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="1">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1">
+      <c r="F28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -1645,26 +1394,26 @@
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1">
+      <c r="F29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -1674,7 +1423,7 @@
       <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1686,95 +1435,95 @@
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="1">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1">
+      <c r="F31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32"/>
+      <c r="B32" s="0"/>
       <c r="C32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="1">
-        <v>2</v>
-      </c>
-      <c r="G32" s="1">
-        <v>20</v>
-      </c>
-      <c r="H32" s="1">
+      <c r="F32" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H32" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="1">
-        <v>2</v>
-      </c>
-      <c r="G33" s="1">
-        <v>20</v>
-      </c>
-      <c r="H33" s="1">
+      <c r="F33" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -1784,26 +1533,26 @@
       <c r="C34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="1" t="n">
         <v>15</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="1">
-        <v>2</v>
-      </c>
-      <c r="G34" s="1">
-        <v>20</v>
-      </c>
-      <c r="H34" s="1">
+      <c r="F34" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H34" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
@@ -1813,26 +1562,26 @@
       <c r="C35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="1">
-        <v>2</v>
-      </c>
-      <c r="G35" s="1">
-        <v>20</v>
-      </c>
-      <c r="H35" s="1">
+      <c r="F35" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
@@ -1842,19 +1591,19 @@
       <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="1">
-        <v>2</v>
-      </c>
-      <c r="G36" s="1">
-        <v>20</v>
-      </c>
-      <c r="H36" s="1">
+      <c r="F36" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H36" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -1862,35 +1611,44 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.796875" style="1"/>
-    <col min="2" max="2" width="13.53125" style="1"/>
-    <col min="3" max="3" width="39.265625" style="1"/>
-    <col min="4" max="4" width="11.46484375" style="1"/>
-    <col min="5" max="5" width="12.1328125" style="1"/>
-    <col min="6" max="6" width="12.19921875" style="1"/>
-    <col min="7" max="7" width="7.265625" style="1"/>
-    <col min="8" max="8" width="15.3984375" style="1"/>
-    <col min="9" max="9" width="11.46484375" style="1"/>
-    <col min="10" max="1025" width="9.06640625" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1336032388664"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1919,61 +1677,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2"/>
+      <c r="B2" s="0"/>
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="F2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3"/>
+      <c r="B3" s="0"/>
       <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="F3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1983,53 +1741,53 @@
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="F4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" s="0"/>
       <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="F5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -2039,134 +1797,134 @@
       <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="F6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7"/>
+      <c r="B7" s="0"/>
       <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="F7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" s="0"/>
       <c r="C8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="F8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9"/>
+      <c r="B9" s="0"/>
       <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="F9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" s="0"/>
       <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1">
+      <c r="F10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -2176,26 +1934,26 @@
       <c r="C11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="F11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -2205,26 +1963,26 @@
       <c r="C12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="F12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -2234,26 +1992,26 @@
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="F13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -2263,26 +2021,26 @@
       <c r="C14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1">
+      <c r="F14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
@@ -2292,26 +2050,26 @@
       <c r="C15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="F15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -2321,26 +2079,26 @@
       <c r="C16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1">
+      <c r="F16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
@@ -2350,26 +2108,26 @@
       <c r="C17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="F17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -2379,26 +2137,26 @@
       <c r="C18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="1" t="n">
         <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="F18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -2408,7 +2166,7 @@
       <c r="C19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="1" t="n">
         <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -2420,14 +2178,14 @@
       <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -2437,7 +2195,7 @@
       <c r="C20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2449,14 +2207,14 @@
       <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -2466,26 +2224,26 @@
       <c r="C21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1">
+      <c r="F21" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <v>0.4</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
         <v>79</v>
       </c>
@@ -2495,26 +2253,26 @@
       <c r="C22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="F22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -2524,26 +2282,26 @@
       <c r="C23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1">
+      <c r="F23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>85</v>
       </c>
@@ -2553,26 +2311,26 @@
       <c r="C24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="1" t="n">
         <v>20</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1">
+      <c r="F24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -2582,26 +2340,26 @@
       <c r="C25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="F25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>87</v>
       </c>
@@ -2611,26 +2369,26 @@
       <c r="C26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="F26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>87</v>
       </c>
@@ -2640,26 +2398,26 @@
       <c r="C27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="1">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="F27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>87</v>
       </c>
@@ -2669,26 +2427,26 @@
       <c r="C28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="1">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1">
+      <c r="F28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>92</v>
       </c>
@@ -2698,26 +2456,26 @@
       <c r="C29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G29" s="1">
-        <v>20</v>
-      </c>
-      <c r="H29" s="1">
+      <c r="G29" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H29" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
@@ -2727,26 +2485,26 @@
       <c r="C30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="1">
-        <v>2</v>
-      </c>
-      <c r="G30" s="1">
-        <v>20</v>
-      </c>
-      <c r="H30" s="1">
+      <c r="F30" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H30" s="1" t="n">
         <v>0.4</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -2756,19 +2514,19 @@
       <c r="C31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="1" t="n">
         <v>200</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="1">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1">
+      <c r="F31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -2776,36 +2534,44 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.796875" style="1"/>
-    <col min="2" max="2" width="14" style="1"/>
-    <col min="3" max="3" width="39.265625" style="1"/>
-    <col min="4" max="4" width="9.06640625" style="1"/>
-    <col min="5" max="5" width="7.53125" style="1"/>
-    <col min="6" max="6" width="12.59765625" style="1"/>
-    <col min="7" max="7" width="7.3984375" style="1"/>
-    <col min="8" max="8" width="15.796875" style="1"/>
-    <col min="9" max="9" width="19.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="1025" width="9.06640625" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.52631578947368"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.5991902834008"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.39676113360324"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7975708502024"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.1943319838057"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2834,7 +2600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>97</v>
       </c>
@@ -2844,26 +2610,26 @@
       <c r="C2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="F2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -2873,26 +2639,26 @@
       <c r="C3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="F3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
@@ -2902,26 +2668,26 @@
       <c r="C4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="F4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>105</v>
       </c>
@@ -2931,55 +2697,55 @@
       <c r="C5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="1">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="F5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="1">
+        <v>109</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="F6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -2987,550 +2753,550 @@
         <v>107</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="1">
+        <v>110</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="F7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="1">
+        <v>111</v>
+      </c>
+      <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="F8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D9" s="1">
+        <v>113</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="F9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F11" s="1">
-        <v>4</v>
-      </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="1">
-        <v>3</v>
-      </c>
-      <c r="G12" s="1">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="1">
-        <v>4</v>
-      </c>
-      <c r="G17" s="1">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="1">
-        <v>4</v>
-      </c>
-      <c r="G18" s="1">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2</v>
-      </c>
-      <c r="G19" s="1">
-        <v>20</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A20" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" s="1">
+        <v>128</v>
+      </c>
+      <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="1">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1">
+      <c r="F20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <v>0.2</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F21" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="1">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="1">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -3542,12 +3308,248 @@
       <c r="G27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.6"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.52631578947368"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.5991902834008"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.39676113360324"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7975708502024"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.1943319838057"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished LA and PA models for modular hearts.  Started request for more equipment tray holders
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683F73FE-3F70-4232-AA3D-0F5E3E5516E5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="May 2018" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="June 2018" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="July 2018" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="August 2018" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="May 2018" sheetId="1" r:id="rId1"/>
+    <sheet name="June 2018" sheetId="2" r:id="rId2"/>
+    <sheet name="July 2018" sheetId="3" r:id="rId3"/>
+    <sheet name="August 2018" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="141">
   <si>
     <t>Date Requested</t>
   </si>
@@ -435,18 +441,22 @@
   </si>
   <si>
     <t>01-08-2018</t>
+  </si>
+  <si>
+    <t>03-08-2018</t>
+  </si>
+  <si>
+    <t>02-08-2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="DD/MMM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -455,22 +465,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -487,7 +482,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -495,96 +490,362 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK36"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.39676113360324"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="13.53125" style="1"/>
+    <col min="3" max="3" width="36.06640625" style="1"/>
+    <col min="4" max="4" width="11.46484375" style="1"/>
+    <col min="5" max="5" width="9.3984375" style="1"/>
+    <col min="6" max="6" width="12.19921875" style="1"/>
+    <col min="7" max="7" width="7.265625" style="1"/>
+    <col min="8" max="8" width="15.3984375" style="1"/>
+    <col min="9" max="9" width="11.46484375" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -613,17 +874,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="3">
         <v>43224</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="3">
         <v>43224</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -635,24 +896,24 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1">
         <v>0.1</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="3">
         <v>43224</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="3">
         <v>43225</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -664,24 +925,24 @@
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="1">
         <v>0.1</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="3">
         <v>43224</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="3">
         <v>43225</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -693,24 +954,24 @@
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="1">
         <v>0.1</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="3">
         <v>43224</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="3">
         <v>43226</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -722,24 +983,24 @@
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="1">
         <v>0.1</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="3">
         <v>43224</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="3">
         <v>43227</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -751,24 +1012,24 @@
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="1">
         <v>0.1</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="3">
         <v>43224</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="3">
         <v>43228</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -780,24 +1041,24 @@
       <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="1">
         <v>0.1</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="3">
         <v>43224</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="3">
         <v>43242</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -809,15 +1070,15 @@
       <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="1">
         <v>0.1</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="3">
         <v>43224</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -826,7 +1087,7 @@
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -838,15 +1099,15 @@
       <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H9" s="1">
         <v>0.1</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="3">
         <v>43224</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -855,7 +1116,7 @@
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -867,160 +1128,160 @@
       <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="1">
         <v>0.1</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="3">
         <v>43238</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="3">
         <v>43242</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="3">
         <v>43238</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="3">
         <v>43242</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="3">
         <v>43238</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="3">
         <v>43242</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="3">
         <v>43238</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="3">
         <v>43242</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="n">
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
         <v>100</v>
       </c>
-      <c r="H14" s="1" t="n">
+      <c r="H14" s="1">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="3">
         <v>43238</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="3">
         <v>43242</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="3">
         <v>43242</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1029,27 +1290,27 @@
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1" t="n">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="3">
         <v>43242</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1058,27 +1319,27 @@
       <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1" t="n">
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="3">
         <v>43242</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1087,26 +1348,26 @@
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="n">
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1116,53 +1377,53 @@
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" s="1" t="n">
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
         <v>100</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="1">
         <v>0.2</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="0"/>
+      <c r="B20"/>
       <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="1">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="n">
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1">
         <v>0.2</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -1172,161 +1433,161 @@
       <c r="C21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="n">
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
         <v>0.2</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="0"/>
+      <c r="B22"/>
       <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="n">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="0"/>
+      <c r="B23"/>
       <c r="C23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="1">
         <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="n">
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="0"/>
+      <c r="B24"/>
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="1">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1" t="n">
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="0"/>
+      <c r="B25"/>
       <c r="C25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="1">
         <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1" t="n">
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="0"/>
+      <c r="B26"/>
       <c r="C26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="1">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1" t="n">
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1336,26 +1597,26 @@
       <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="1">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1" t="n">
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1365,26 +1626,26 @@
       <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="1">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1" t="n">
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -1394,26 +1655,26 @@
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1" t="n">
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
         <v>10</v>
       </c>
-      <c r="H29" s="1" t="n">
+      <c r="H29" s="1">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -1423,7 +1684,7 @@
       <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1435,95 +1696,95 @@
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="1" t="n">
+      <c r="H30" s="1">
         <v>0.2</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="0"/>
+      <c r="B31"/>
       <c r="C31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="D31" s="1">
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1" t="n">
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="0"/>
+      <c r="B32"/>
       <c r="C32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="1" t="n">
+      <c r="D32" s="1">
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G32" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H32" s="1" t="n">
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>20</v>
+      </c>
+      <c r="H32" s="1">
         <v>0.2</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="0"/>
+      <c r="B33"/>
       <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="1" t="n">
+      <c r="D33" s="1">
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H33" s="1" t="n">
+      <c r="F33" s="1">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1">
         <v>0.2</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -1533,26 +1794,26 @@
       <c r="C34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="1" t="n">
+      <c r="D34" s="1">
         <v>15</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G34" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H34" s="1" t="n">
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>20</v>
+      </c>
+      <c r="H34" s="1">
         <v>0.2</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
@@ -1562,26 +1823,26 @@
       <c r="C35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="1" t="n">
+      <c r="D35" s="1">
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H35" s="1" t="n">
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1">
         <v>0.2</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
@@ -1591,19 +1852,19 @@
       <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="1" t="n">
+      <c r="D36" s="1">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G36" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H36" s="1" t="n">
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>20</v>
+      </c>
+      <c r="H36" s="1">
         <v>0.2</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -1611,44 +1872,35 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMK31"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1336032388664"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.27125506072875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="13.53125" style="1"/>
+    <col min="3" max="3" width="39.265625" style="1"/>
+    <col min="4" max="4" width="11.46484375" style="1"/>
+    <col min="5" max="5" width="12.1328125" style="1"/>
+    <col min="6" max="6" width="12.19921875" style="1"/>
+    <col min="7" max="7" width="7.265625" style="1"/>
+    <col min="8" max="8" width="15.3984375" style="1"/>
+    <col min="9" max="9" width="11.46484375" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1677,61 +1929,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="0"/>
+      <c r="B2"/>
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="0"/>
+      <c r="B3"/>
       <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1741,53 +1993,53 @@
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="n">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="0"/>
+      <c r="B5"/>
       <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1" t="n">
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1797,134 +2049,134 @@
       <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1" t="n">
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="0"/>
+      <c r="B7"/>
       <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="n">
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
         <v>0.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="0"/>
+      <c r="B8"/>
       <c r="C8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1" t="n">
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1">
         <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="0"/>
+      <c r="B9"/>
       <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1" t="n">
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1">
         <v>0.2</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="0"/>
+      <c r="B10"/>
       <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1" t="n">
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1">
         <v>0.2</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -1934,26 +2186,26 @@
       <c r="C11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -1963,26 +2215,26 @@
       <c r="C12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -1992,26 +2244,26 @@
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -2021,26 +2273,26 @@
       <c r="C14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1" t="n">
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
@@ -2050,26 +2302,26 @@
       <c r="C15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>4</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -2079,26 +2331,26 @@
       <c r="C16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1" t="n">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
@@ -2108,26 +2360,26 @@
       <c r="C17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1" t="n">
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -2137,26 +2389,26 @@
       <c r="C18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="n">
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -2166,7 +2418,7 @@
       <c r="C19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -2178,14 +2430,14 @@
       <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="1">
         <v>0.1</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -2195,7 +2447,7 @@
       <c r="C20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2207,14 +2459,14 @@
       <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="H20" s="1">
         <v>0.1</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -2224,26 +2476,26 @@
       <c r="C21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="n">
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
         <v>0.4</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
         <v>79</v>
       </c>
@@ -2253,26 +2505,26 @@
       <c r="C22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="n">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
         <v>0.2</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -2282,26 +2534,26 @@
       <c r="C23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="1">
         <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="n">
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
         <v>0.2</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>85</v>
       </c>
@@ -2311,26 +2563,26 @@
       <c r="C24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="1">
         <v>20</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1" t="n">
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
         <v>0.2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -2340,26 +2592,26 @@
       <c r="C25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="1">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1" t="n">
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
         <v>0.2</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>87</v>
       </c>
@@ -2369,26 +2621,26 @@
       <c r="C26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="1">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1" t="n">
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
         <v>0.2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>87</v>
       </c>
@@ -2398,26 +2650,26 @@
       <c r="C27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="1">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H27" s="1" t="n">
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1">
         <v>0.2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>87</v>
       </c>
@@ -2427,26 +2679,26 @@
       <c r="C28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="1">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1" t="n">
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1">
         <v>0.2</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>92</v>
       </c>
@@ -2456,26 +2708,26 @@
       <c r="C29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D29" s="1">
         <v>4</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="1" t="n">
+      <c r="F29" s="1">
         <v>3</v>
       </c>
-      <c r="G29" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H29" s="1" t="n">
+      <c r="G29" s="1">
+        <v>20</v>
+      </c>
+      <c r="H29" s="1">
         <v>0.2</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
@@ -2485,26 +2737,26 @@
       <c r="C30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G30" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H30" s="1" t="n">
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>20</v>
+      </c>
+      <c r="H30" s="1">
         <v>0.4</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -2514,19 +2766,19 @@
       <c r="C31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="D31" s="1">
         <v>200</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1" t="n">
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1">
         <v>0.2</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -2534,44 +2786,36 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AMK27"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView windowProtection="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9959514170041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.52631578947368"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.5991902834008"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.39676113360324"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7975708502024"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.1943319838057"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="14" style="1"/>
+    <col min="3" max="3" width="39.265625" style="1"/>
+    <col min="4" max="4" width="9.06640625" style="1"/>
+    <col min="5" max="5" width="7.53125" style="1"/>
+    <col min="6" max="6" width="12.59765625" style="1"/>
+    <col min="7" max="7" width="7.3984375" style="1"/>
+    <col min="8" max="8" width="15.796875" style="1"/>
+    <col min="9" max="9" width="19.19921875" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2600,7 +2844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>97</v>
       </c>
@@ -2610,26 +2854,26 @@
       <c r="C2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -2639,26 +2883,26 @@
       <c r="C3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
         <v>0.2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
@@ -2668,26 +2912,26 @@
       <c r="C4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="n">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>105</v>
       </c>
@@ -2697,26 +2941,26 @@
       <c r="C5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1" t="n">
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>107</v>
       </c>
@@ -2726,26 +2970,26 @@
       <c r="C6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1" t="n">
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -2755,26 +2999,26 @@
       <c r="C7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="n">
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
         <v>0.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>107</v>
       </c>
@@ -2784,26 +3028,26 @@
       <c r="C8" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1" t="n">
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1">
         <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>107</v>
       </c>
@@ -2813,26 +3057,26 @@
       <c r="C9" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1" t="n">
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1">
         <v>0.2</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>107</v>
       </c>
@@ -2842,26 +3086,26 @@
       <c r="C10" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1" t="n">
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1">
         <v>0.2</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>114</v>
       </c>
@@ -2871,26 +3115,26 @@
       <c r="C11" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="F11" s="1">
         <v>4</v>
       </c>
-      <c r="G11" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>114</v>
       </c>
@@ -2900,26 +3144,26 @@
       <c r="C12" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="1">
         <v>3</v>
       </c>
-      <c r="G12" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.2</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>114</v>
       </c>
@@ -2929,26 +3173,26 @@
       <c r="C13" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>114</v>
       </c>
@@ -2958,26 +3202,26 @@
       <c r="C14" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1" t="n">
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>121</v>
       </c>
@@ -2987,26 +3231,26 @@
       <c r="C15" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>121</v>
       </c>
@@ -3016,26 +3260,26 @@
       <c r="C16" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1" t="n">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.2</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>112</v>
       </c>
@@ -3045,26 +3289,26 @@
       <c r="C17" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="n">
+      <c r="F17" s="1">
         <v>4</v>
       </c>
-      <c r="G17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1" t="n">
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>112</v>
       </c>
@@ -3074,26 +3318,26 @@
       <c r="C18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="1" t="n">
+      <c r="F18" s="1">
         <v>4</v>
       </c>
-      <c r="G18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="n">
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
         <v>0.2</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
@@ -3103,26 +3347,26 @@
       <c r="C19" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H19" s="1" t="n">
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>20</v>
+      </c>
+      <c r="H19" s="1">
         <v>0.2</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>112</v>
       </c>
@@ -3132,171 +3376,171 @@
       <c r="C20" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="n">
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1">
         <v>0.2</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="1">
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="1">
         <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="1">
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="1">
         <v>10</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H25" s="1" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="1">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="1">
         <v>10</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -3308,49 +3552,40 @@
       <c r="G27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="1" t="n">
+      <c r="H27" s="1">
         <v>0.2</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AMK10"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.6"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9959514170041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.2712550607287"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.52631578947368"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.5991902834008"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.39676113360324"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7975708502024"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.1943319838057"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.06072874493927"/>
+    <col min="1" max="1" width="13.796875" style="1"/>
+    <col min="2" max="2" width="14" style="1"/>
+    <col min="3" max="3" width="39.265625" style="1"/>
+    <col min="4" max="4" width="9.06640625" style="1"/>
+    <col min="5" max="5" width="7.53125" style="1"/>
+    <col min="6" max="6" width="12.59765625" style="1"/>
+    <col min="7" max="7" width="7.3984375" style="1"/>
+    <col min="8" max="8" width="15.796875" style="1"/>
+    <col min="9" max="9" width="19.19921875" style="1"/>
+    <col min="10" max="1025" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3379,76 +3614,79 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>130</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>130</v>
       </c>
@@ -3458,76 +3696,79 @@
       <c r="C5" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>130</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -3539,17 +3780,58 @@
       <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1">
         <v>0.2</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new request for evhp concept 6 part and fixed incorrect material types for July and Aug prints
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED022A94-FD81-4EB2-A8E4-EB4C353D83C4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0289BB65-884C-40C6-8DBF-C31BD535CB28}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="May 2018" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="143">
   <si>
     <t>Date Requested</t>
   </si>
@@ -447,6 +447,12 @@
   </si>
   <si>
     <t>02-08-2018</t>
+  </si>
+  <si>
+    <t>06-08-2018</t>
+  </si>
+  <si>
+    <t>EVHP Holder TEE Track Concept 6</t>
   </si>
 </sst>
 </file>
@@ -2795,10 +2801,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK27"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3380,7 +3386,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F20" s="1">
         <v>2</v>
@@ -3406,7 +3412,7 @@
         <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
@@ -3429,7 +3435,7 @@
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F22" s="1">
         <v>2</v>
@@ -3452,7 +3458,7 @@
         <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
@@ -3475,7 +3481,7 @@
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F24" s="1">
         <v>2</v>
@@ -3498,7 +3504,7 @@
         <v>10</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F25" s="1">
         <v>2</v>
@@ -3521,7 +3527,7 @@
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F26" s="1">
         <v>2</v>
@@ -3564,11 +3570,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK10"/>
+  <dimension ref="A1:AMK11"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3625,7 +3631,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1">
         <v>2</v>
@@ -3651,7 +3657,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -3674,7 +3680,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1">
         <v>2</v>
@@ -3700,7 +3706,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
@@ -3726,7 +3732,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
@@ -3752,7 +3758,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
@@ -3798,7 +3804,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F9" s="1">
         <v>3</v>
@@ -3821,7 +3827,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1">
         <v>3</v>
@@ -3830,6 +3836,29 @@
         <v>20</v>
       </c>
       <c r="H10" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated completed prints and added new tee spacer and equipment holder clip
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0289BB65-884C-40C6-8DBF-C31BD535CB28}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F030186-AF78-4E64-900A-70F3E963BEA7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="May 2018" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="146">
   <si>
     <t>Date Requested</t>
   </si>
@@ -453,6 +453,15 @@
   </si>
   <si>
     <t>EVHP Holder TEE Track Concept 6</t>
+  </si>
+  <si>
+    <t>07-08-2018</t>
+  </si>
+  <si>
+    <t>Mini TEE Spacer</t>
+  </si>
+  <si>
+    <t>09-09-2018</t>
   </si>
 </sst>
 </file>
@@ -2801,7 +2810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK27"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="E19" sqref="E19:E26"/>
@@ -3570,11 +3579,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK11"/>
+  <dimension ref="A1:AMK13"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3797,6 +3806,9 @@
       <c r="A9" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>125</v>
       </c>
@@ -3820,6 +3832,9 @@
       <c r="A10" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>126</v>
       </c>
@@ -3843,6 +3858,9 @@
       <c r="A11" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>142</v>
       </c>
@@ -3859,6 +3877,58 @@
         <v>20</v>
       </c>
       <c r="H11" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="1">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added experiment for spine box casting case with htpla
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F030186-AF78-4E64-900A-70F3E963BEA7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F5D9F4-9EFB-4DC6-9279-3DA866BA0920}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="148">
   <si>
     <t>Date Requested</t>
   </si>
@@ -462,6 +462,12 @@
   </si>
   <si>
     <t>09-09-2018</t>
+  </si>
+  <si>
+    <t>Spine Box 3lvl Casting Case</t>
+  </si>
+  <si>
+    <t>HTPLA</t>
   </si>
 </sst>
 </file>
@@ -3579,11 +3585,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK13"/>
+  <dimension ref="A1:AMK14"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3932,6 +3938,29 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
request for evhp concept 5 replacement part
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F5D9F4-9EFB-4DC6-9279-3DA866BA0920}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3780EF-F263-4141-955E-6FF541309421}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="149">
   <si>
     <t>Date Requested</t>
   </si>
@@ -468,6 +468,9 @@
   </si>
   <si>
     <t>HTPLA</t>
+  </si>
+  <si>
+    <t>EVHP TEE Track Connector v3</t>
   </si>
 </sst>
 </file>
@@ -3585,11 +3588,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK14"/>
+  <dimension ref="A1:AMK15"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3961,6 +3964,29 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
fixed incorrect dates and added more prints for the spine box
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3780EF-F263-4141-955E-6FF541309421}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F160ED-5A58-41D7-B691-1AC6D09EDAE5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="151">
   <si>
     <t>Date Requested</t>
   </si>
@@ -461,9 +461,6 @@
     <t>Mini TEE Spacer</t>
   </si>
   <si>
-    <t>09-09-2018</t>
-  </si>
-  <si>
     <t>Spine Box 3lvl Casting Case</t>
   </si>
   <si>
@@ -471,6 +468,15 @@
   </si>
   <si>
     <t>EVHP TEE Track Connector v3</t>
+  </si>
+  <si>
+    <t>09-08-2018</t>
+  </si>
+  <si>
+    <t>10-08-2018</t>
+  </si>
+  <si>
+    <t>Spine Box 3lvl Lumbar Spine</t>
   </si>
 </sst>
 </file>
@@ -3588,11 +3594,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK15"/>
+  <dimension ref="A1:AMK16"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3891,10 +3897,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>144</v>
@@ -3917,10 +3923,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>123</v>
@@ -3943,16 +3949,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="F14" s="1">
         <v>2</v>
@@ -3966,10 +3975,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -3984,6 +3993,29 @@
         <v>20</v>
       </c>
       <c r="H15" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reprinting the casting case with bridge, lumbar spine and track connector completed
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F160ED-5A58-41D7-B691-1AC6D09EDAE5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF902E2-E6B4-46F1-BD1A-0989517F4CB0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="151">
   <si>
     <t>Date Requested</t>
   </si>
@@ -3594,11 +3594,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK16"/>
+  <dimension ref="A1:AMK17"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3977,6 +3977,9 @@
       <c r="A15" s="1" t="s">
         <v>148</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>147</v>
       </c>
@@ -4000,6 +4003,9 @@
       <c r="A16" s="1" t="s">
         <v>149</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>150</v>
       </c>
@@ -4016,6 +4022,29 @@
         <v>20</v>
       </c>
       <c r="H16" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
printing mold pieces for parametric Ao (test)
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF902E2-E6B4-46F1-BD1A-0989517F4CB0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73BB770-10C4-4C0E-A918-D321F94EAB45}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="152">
   <si>
     <t>Date Requested</t>
   </si>
@@ -477,6 +477,9 @@
   </si>
   <si>
     <t>Spine Box 3lvl Lumbar Spine</t>
+  </si>
+  <si>
+    <t>Parametric Ao Test Mold</t>
   </si>
 </sst>
 </file>
@@ -3594,11 +3597,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK17"/>
+  <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4048,6 +4051,29 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
completed the test mold and nylon casting case
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73BB770-10C4-4C0E-A918-D321F94EAB45}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87719E68-0957-4B67-9F1B-FAEF29C047BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="153">
   <si>
     <t>Date Requested</t>
   </si>
@@ -480,6 +480,9 @@
   </si>
   <si>
     <t>Parametric Ao Test Mold</t>
+  </si>
+  <si>
+    <t>11-02-2018</t>
   </si>
 </sst>
 </file>
@@ -3601,7 +3604,7 @@
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4032,6 +4035,9 @@
       <c r="A17" s="1" t="s">
         <v>149</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>145</v>
       </c>
@@ -4054,6 +4060,9 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>149</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
prints for TEE controller
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87719E68-0957-4B67-9F1B-FAEF29C047BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2715531F-0556-442D-947B-9EF2338946FA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="158">
   <si>
     <t>Date Requested</t>
   </si>
@@ -483,6 +483,21 @@
   </si>
   <si>
     <t>11-02-2018</t>
+  </si>
+  <si>
+    <t>13-08-2018</t>
+  </si>
+  <si>
+    <t>TEE Controller v2 - misc pieces</t>
+  </si>
+  <si>
+    <t>14-08-2018</t>
+  </si>
+  <si>
+    <t>TEE Controller v2 - Top</t>
+  </si>
+  <si>
+    <t>TEE Controller v2 - Bot</t>
   </si>
 </sst>
 </file>
@@ -3600,11 +3615,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK18"/>
+  <dimension ref="A1:AMK21"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4083,6 +4098,78 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1">
+        <v>20</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="1">
+        <v>4</v>
+      </c>
+      <c r="G20" s="1">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
completed TEE v2 pieces
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2715531F-0556-442D-947B-9EF2338946FA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88E9509-95E4-482A-8CDE-A664027274A3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="158">
   <si>
     <t>Date Requested</t>
   </si>
@@ -3619,7 +3619,7 @@
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4128,6 +4128,9 @@
       <c r="A20" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>156</v>
       </c>
@@ -4149,6 +4152,9 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C21" s="1" t="s">

</xml_diff>

<commit_message>
added request for 50 scale FOCUS set
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88E9509-95E4-482A-8CDE-A664027274A3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247CFD8F-3FA1-4392-83A6-884E6033DA62}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="163">
   <si>
     <t>Date Requested</t>
   </si>
@@ -498,6 +498,21 @@
   </si>
   <si>
     <t>TEE Controller v2 - Bot</t>
+  </si>
+  <si>
+    <t>16-08-2018</t>
+  </si>
+  <si>
+    <t>FOCUS Box bot</t>
+  </si>
+  <si>
+    <t>50 scale LAX</t>
+  </si>
+  <si>
+    <t>50 scale SAX</t>
+  </si>
+  <si>
+    <t>FOCUS Box tops</t>
   </si>
 </sst>
 </file>
@@ -3615,11 +3630,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK21"/>
+  <dimension ref="A1:AMK25"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4176,6 +4191,101 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
updated focus box top completion, papvc request, fixed some layer height errors
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247CFD8F-3FA1-4392-83A6-884E6033DA62}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF9CF18-59BB-4170-85F6-FE5E6205ECAD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="165">
   <si>
     <t>Date Requested</t>
   </si>
@@ -513,6 +513,12 @@
   </si>
   <si>
     <t>FOCUS Box tops</t>
+  </si>
+  <si>
+    <t>19-08-2018</t>
+  </si>
+  <si>
+    <t>papvc model</t>
   </si>
 </sst>
 </file>
@@ -3630,11 +3636,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK25"/>
+  <dimension ref="A1:AMK26"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3850,7 +3856,7 @@
         <v>11</v>
       </c>
       <c r="H8" s="1">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -4267,6 +4273,9 @@
       <c r="A25" s="1" t="s">
         <v>158</v>
       </c>
+      <c r="B25" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="C25" s="1" t="s">
         <v>162</v>
       </c>
@@ -4284,6 +4293,29 @@
       </c>
       <c r="H25" s="1">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed LAX SAX and papvc models
</commit_message>
<xml_diff>
--- a/print_request_logsheet.xlsx
+++ b/print_request_logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Print Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF9CF18-59BB-4170-85F6-FE5E6205ECAD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF39A00-553C-41E7-9523-D60582D74846}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="166">
   <si>
     <t>Date Requested</t>
   </si>
@@ -519,6 +519,9 @@
   </si>
   <si>
     <t>papvc model</t>
+  </si>
+  <si>
+    <t>20-08-2018</t>
   </si>
 </sst>
 </file>
@@ -3640,7 +3643,7 @@
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4227,6 +4230,9 @@
       <c r="A23" s="1" t="s">
         <v>158</v>
       </c>
+      <c r="B23" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>160</v>
       </c>
@@ -4250,6 +4256,9 @@
       <c r="A24" s="1" t="s">
         <v>158</v>
       </c>
+      <c r="B24" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>161</v>
       </c>
@@ -4298,6 +4307,9 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>163</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>164</v>

</xml_diff>